<commit_message>
functions9 - different functions
</commit_message>
<xml_diff>
--- a/001EffortTracker/KT Plan.xlsx
+++ b/001EffortTracker/KT Plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="284">
   <si>
     <t>Playwright: Web Automation Testing From Zero to Hero - Artem Bondar</t>
   </si>
@@ -497,6 +497,23 @@
   </si>
   <si>
     <t>Revision Day 6</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch 1 video then practise it perfectly by writing notes and trying 
+on editor  </t>
+  </si>
+  <si>
+    <t>Revise previous days topics Next days</t>
+  </si>
+  <si>
+    <t>Practise more programs outside the course aswel, 
+Generate your own programs and scenarios and try to implement it</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>JavaScript - YouTube - NaveenAutoLabs</t>
@@ -970,7 +987,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1072,6 +1089,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
@@ -1431,10 +1463,10 @@
     <col min="2" max="2" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="49" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="47" width="38.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="47" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="47" width="41.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="54" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="52" width="38.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="52" width="25.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="52" width="41.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1443,9 +1475,9 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="21"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="22"/>
@@ -1456,10 +1488,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>6</v>
@@ -1474,10 +1506,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="H3" s="17"/>
     </row>
@@ -1490,10 +1522,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="H4" s="17"/>
     </row>
@@ -1506,10 +1538,10 @@
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="H5" s="17"/>
     </row>
@@ -1525,7 +1557,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H6" s="17"/>
     </row>
@@ -1538,13 +1570,13 @@
         <v>5</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="H7" s="48" t="s">
-        <v>262</v>
+        <v>265</v>
+      </c>
+      <c r="H7" s="53" t="s">
+        <v>267</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -1556,10 +1588,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="H8" s="17"/>
     </row>
@@ -1572,10 +1604,10 @@
         <v>7</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="H9" s="17"/>
     </row>
@@ -1588,10 +1620,10 @@
         <v>8</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="H10" s="17"/>
     </row>
@@ -1604,10 +1636,10 @@
         <v>9</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="H11" s="17"/>
     </row>
@@ -1620,10 +1652,10 @@
         <v>10</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H12" s="17"/>
     </row>
@@ -1636,10 +1668,10 @@
         <v>11</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H13" s="17"/>
     </row>
@@ -1652,10 +1684,10 @@
         <v>12</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H14" s="17"/>
     </row>
@@ -1668,13 +1700,13 @@
         <v>13</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="H15" s="48" t="s">
-        <v>273</v>
+        <v>277</v>
+      </c>
+      <c r="H15" s="53" t="s">
+        <v>278</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
@@ -1686,13 +1718,13 @@
         <v>14</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="H16" s="48" t="s">
-        <v>275</v>
+        <v>277</v>
+      </c>
+      <c r="H16" s="53" t="s">
+        <v>280</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
@@ -1704,13 +1736,13 @@
         <v>15</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="H17" s="48" t="s">
         <v>277</v>
+      </c>
+      <c r="H17" s="53" t="s">
+        <v>282</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
@@ -1722,10 +1754,10 @@
         <v>16</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="H18" s="17"/>
     </row>
@@ -1749,2625 +1781,2688 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G198"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="23" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="47" width="37.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="52" width="60.29071428571429" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="33" width="8.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="34" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="47" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="47" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="47" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="52" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="52" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="52" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="35" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="35"/>
+      <c r="B1" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="36"/>
       <c r="C1" s="37"/>
       <c r="D1" s="38"/>
       <c r="E1" s="36"/>
       <c r="F1" s="36"/>
-      <c r="G1" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="13" t="s">
+      <c r="G1" s="36"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="31.5">
+      <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="35">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="B3" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5">
+      <c r="A4" s="35">
         <v>3</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="B4" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="35"/>
+      <c r="B5" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="46.5">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="29">
-        <v>8.03</v>
-      </c>
-      <c r="D3" s="18">
-        <v>45355</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="15">
-        <v>2</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="29">
-        <v>20.56</v>
-      </c>
-      <c r="D4" s="18">
-        <v>45355</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33">
-      <c r="A5" s="15">
-        <v>3</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" s="29">
-        <v>34.45</v>
-      </c>
-      <c r="D5" s="18">
-        <v>45355</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="40" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="46.5">
-      <c r="A6" s="15">
-        <v>4</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="C6" s="29">
-        <v>32.53</v>
-      </c>
-      <c r="D6" s="18">
-        <v>45356</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="33">
-      <c r="A7" s="15">
-        <v>5</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" s="29">
-        <v>28.2</v>
-      </c>
-      <c r="D7" s="18">
-        <v>45356</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="39"/>
+      <c r="G7" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33">
       <c r="A8" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="29">
+        <v>8.03</v>
+      </c>
+      <c r="D8" s="18">
+        <v>45355</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="15">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="C8" s="29">
-        <v>32.09</v>
-      </c>
-      <c r="D8" s="18">
-        <v>45357</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="33">
-      <c r="A9" s="15">
-        <v>7</v>
-      </c>
-      <c r="B9" s="16" t="s">
+      <c r="C9" s="29">
+        <v>20.56</v>
+      </c>
+      <c r="D9" s="18">
+        <v>45355</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="15">
+        <v>3</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="29">
-        <v>15.04</v>
-      </c>
-      <c r="D9" s="18">
-        <v>45357</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33">
-      <c r="A10" s="15">
-        <v>8</v>
-      </c>
-      <c r="B10" s="16" t="s">
+      <c r="C10" s="29">
+        <v>34.45</v>
+      </c>
+      <c r="D10" s="18">
+        <v>45355</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="29">
-        <v>29.46</v>
-      </c>
-      <c r="D10" s="18">
-        <v>45358</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="39"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="33">
       <c r="A11" s="15">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>170</v>
       </c>
       <c r="C11" s="29">
-        <v>26.4</v>
+        <v>32.53</v>
       </c>
       <c r="D11" s="18">
-        <v>45358</v>
-      </c>
-      <c r="E11" s="17"/>
+        <v>45356</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>166</v>
+      </c>
       <c r="F11" s="17"/>
-      <c r="G11" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="33">
+      <c r="G11" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>171</v>
       </c>
       <c r="C12" s="29">
-        <v>24.52</v>
+        <v>28.2</v>
       </c>
       <c r="D12" s="18">
-        <v>45359</v>
-      </c>
-      <c r="E12" s="17"/>
+        <v>45356</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>166</v>
+      </c>
       <c r="F12" s="17"/>
-      <c r="G12" s="39"/>
+      <c r="G12" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="15">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>172</v>
       </c>
       <c r="C13" s="29">
-        <v>7.19</v>
+        <v>32.09</v>
       </c>
       <c r="D13" s="18">
-        <v>45359</v>
-      </c>
-      <c r="E13" s="17"/>
+        <v>45357</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>166</v>
+      </c>
       <c r="F13" s="17"/>
-      <c r="G13" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="33">
+      <c r="G13" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="15">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>173</v>
       </c>
       <c r="C14" s="29">
-        <v>13.33</v>
+        <v>15.04</v>
       </c>
       <c r="D14" s="18">
-        <v>45359</v>
-      </c>
-      <c r="E14" s="17"/>
+        <v>45357</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>166</v>
+      </c>
       <c r="F14" s="17"/>
-      <c r="G14" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="G14" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="15">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>174</v>
       </c>
       <c r="C15" s="29">
-        <v>19.1</v>
+        <v>29.46</v>
       </c>
       <c r="D15" s="18">
-        <v>45359</v>
-      </c>
-      <c r="E15" s="17"/>
+        <v>45358</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>166</v>
+      </c>
       <c r="F15" s="17"/>
-      <c r="G15" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="G15" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="15">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>175</v>
       </c>
       <c r="C16" s="29">
-        <v>25.43</v>
+        <v>26.4</v>
       </c>
       <c r="D16" s="18">
-        <v>45360</v>
+        <v>45358</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="G16" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="15">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="29">
-        <v>37.1</v>
+        <v>24.52</v>
       </c>
       <c r="D17" s="18">
-        <v>45360</v>
+        <v>45359</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="G17" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="15">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>177</v>
       </c>
       <c r="C18" s="29">
-        <v>19.22</v>
+        <v>7.19</v>
       </c>
       <c r="D18" s="18">
-        <v>45361</v>
+        <v>45359</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
-      <c r="G18" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="G18" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="15">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>178</v>
       </c>
       <c r="C19" s="29">
-        <v>9.48</v>
+        <v>13.33</v>
       </c>
       <c r="D19" s="18">
-        <v>45361</v>
+        <v>45359</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
-      <c r="G19" s="39"/>
+      <c r="G19" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="15">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>179</v>
       </c>
       <c r="C20" s="29">
-        <v>22.52</v>
+        <v>19.1</v>
       </c>
       <c r="D20" s="18">
-        <v>45361</v>
+        <v>45359</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="39"/>
+      <c r="G20" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="15">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>180</v>
       </c>
       <c r="C21" s="29">
-        <v>10.07</v>
+        <v>25.43</v>
       </c>
       <c r="D21" s="18">
-        <v>45361</v>
+        <v>45360</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
-      <c r="G21" s="39"/>
+      <c r="G21" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="15">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>181</v>
       </c>
       <c r="C22" s="29">
-        <v>18.28</v>
+        <v>37.1</v>
       </c>
       <c r="D22" s="18">
-        <v>45362</v>
+        <v>45360</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
-      <c r="G22" s="39"/>
+      <c r="G22" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="15">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>182</v>
       </c>
       <c r="C23" s="29">
-        <v>16.07</v>
+        <v>19.22</v>
       </c>
       <c r="D23" s="18">
-        <v>45362</v>
+        <v>45361</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
-      <c r="G23" s="39"/>
+      <c r="G23" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="15">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>183</v>
       </c>
       <c r="C24" s="29">
-        <v>12.29</v>
+        <v>9.48</v>
       </c>
       <c r="D24" s="18">
-        <v>45362</v>
+        <v>45361</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="39"/>
+      <c r="G24" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="15">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>184</v>
       </c>
       <c r="C25" s="29">
-        <v>13.4</v>
+        <v>22.52</v>
       </c>
       <c r="D25" s="18">
-        <v>45362</v>
+        <v>45361</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
-      <c r="G25" s="39"/>
+      <c r="G25" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="15">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>185</v>
       </c>
       <c r="C26" s="29">
-        <v>8.25</v>
+        <v>10.07</v>
       </c>
       <c r="D26" s="18">
-        <v>45363</v>
+        <v>45361</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="39"/>
+      <c r="G26" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="15">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>186</v>
       </c>
       <c r="C27" s="29">
-        <v>5.13</v>
+        <v>18.28</v>
       </c>
       <c r="D27" s="18">
-        <v>45363</v>
+        <v>45362</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
-      <c r="G27" s="39"/>
+      <c r="G27" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="15">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>187</v>
       </c>
       <c r="C28" s="29">
-        <v>6.04</v>
+        <v>16.07</v>
       </c>
       <c r="D28" s="18">
-        <v>45363</v>
+        <v>45362</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
-      <c r="G28" s="39"/>
+      <c r="G28" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="15">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>188</v>
       </c>
       <c r="C29" s="29">
-        <v>6.09</v>
+        <v>12.29</v>
       </c>
       <c r="D29" s="18">
-        <v>45363</v>
+        <v>45362</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
-      <c r="G29" s="39"/>
+      <c r="G29" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="15">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>189</v>
       </c>
       <c r="C30" s="29">
-        <v>12.09</v>
+        <v>13.4</v>
       </c>
       <c r="D30" s="18">
-        <v>45363</v>
+        <v>45362</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
-      <c r="G30" s="39"/>
+      <c r="G30" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="15">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>190</v>
       </c>
       <c r="C31" s="29">
-        <v>12.09</v>
+        <v>8.25</v>
       </c>
       <c r="D31" s="18">
         <v>45363</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
-      <c r="G31" s="39"/>
+      <c r="G31" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="15">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>191</v>
       </c>
       <c r="C32" s="29">
-        <v>25.47</v>
+        <v>5.13</v>
       </c>
       <c r="D32" s="18">
-        <v>45364</v>
+        <v>45363</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
-      <c r="G32" s="39"/>
+      <c r="G32" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="15">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C33" s="29">
-        <v>10.16</v>
+        <v>6.04</v>
       </c>
       <c r="D33" s="18">
-        <v>45364</v>
+        <v>45363</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
-      <c r="G33" s="39"/>
+      <c r="G33" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="15">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>193</v>
       </c>
       <c r="C34" s="29">
-        <v>17.23</v>
+        <v>6.09</v>
       </c>
       <c r="D34" s="18">
-        <v>45364</v>
+        <v>45363</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
-      <c r="G34" s="39"/>
+      <c r="G34" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="15">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>194</v>
       </c>
       <c r="C35" s="29">
-        <v>13.18</v>
+        <v>12.09</v>
       </c>
       <c r="D35" s="18">
-        <v>45364</v>
+        <v>45363</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
-      <c r="G35" s="39"/>
+      <c r="G35" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="15">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>195</v>
       </c>
       <c r="C36" s="29">
-        <v>10.06</v>
+        <v>12.09</v>
       </c>
       <c r="D36" s="18">
-        <v>45365</v>
+        <v>45363</v>
       </c>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
-      <c r="G36" s="39"/>
+      <c r="G36" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="15">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>196</v>
       </c>
       <c r="C37" s="29">
-        <v>2.3</v>
+        <v>25.47</v>
       </c>
       <c r="D37" s="18">
-        <v>45365</v>
+        <v>45364</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
-      <c r="G37" s="39"/>
+      <c r="G37" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="15">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>197</v>
       </c>
       <c r="C38" s="29">
-        <v>14.17</v>
+        <v>10.16</v>
       </c>
       <c r="D38" s="18">
-        <v>45365</v>
+        <v>45364</v>
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
-      <c r="G38" s="39"/>
+      <c r="G38" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="15">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>198</v>
       </c>
       <c r="C39" s="29">
-        <v>27.06</v>
+        <v>17.23</v>
       </c>
       <c r="D39" s="18">
-        <v>45365</v>
+        <v>45364</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
-      <c r="G39" s="39"/>
+      <c r="G39" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="21"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A41" s="11" t="s">
+      <c r="A40" s="15">
+        <v>33</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="2"/>
+      <c r="C40" s="29">
+        <v>13.18</v>
+      </c>
+      <c r="D40" s="18">
+        <v>45364</v>
+      </c>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="A41" s="15">
+        <v>34</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="C41" s="29">
+        <v>10.06</v>
+      </c>
+      <c r="D41" s="18">
+        <v>45365</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G42" s="39"/>
+      <c r="A42" s="15">
+        <v>35</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="29">
+        <v>2.3</v>
+      </c>
+      <c r="D42" s="18">
+        <v>45365</v>
+      </c>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="15">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C43" s="29">
-        <v>17.33</v>
+        <v>14.17</v>
       </c>
       <c r="D43" s="18">
-        <v>45366</v>
+        <v>45365</v>
       </c>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
-      <c r="G43" s="39"/>
+      <c r="G43" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="15">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C44" s="29">
-        <v>18.21</v>
+        <v>27.06</v>
       </c>
       <c r="D44" s="18">
-        <v>45366</v>
+        <v>45365</v>
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
-      <c r="G44" s="39"/>
+      <c r="G44" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="15">
+      <c r="A45" s="21"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A46" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B46" s="12"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="A47" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="C45" s="29">
-        <v>13.01</v>
-      </c>
-      <c r="D45" s="18">
-        <v>45366</v>
-      </c>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="15">
+      <c r="D47" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="C46" s="29">
-        <v>10.17</v>
-      </c>
-      <c r="D46" s="18">
-        <v>45366</v>
-      </c>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="15">
+      <c r="E47" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="C47" s="29">
-        <v>16.56</v>
-      </c>
-      <c r="D47" s="18">
-        <v>45367</v>
-      </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="39"/>
+      <c r="F47" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B48" s="16" t="s">
         <v>205</v>
       </c>
       <c r="C48" s="29">
-        <v>7.56</v>
+        <v>17.33</v>
       </c>
       <c r="D48" s="18">
-        <v>45367</v>
+        <v>45366</v>
       </c>
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
-      <c r="G48" s="39"/>
+      <c r="G48" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>206</v>
       </c>
       <c r="C49" s="29">
-        <v>12.49</v>
+        <v>18.21</v>
       </c>
       <c r="D49" s="18">
-        <v>45367</v>
+        <v>45366</v>
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="17"/>
-      <c r="G49" s="39"/>
+      <c r="G49" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="15">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>207</v>
       </c>
       <c r="C50" s="29">
-        <v>7.13</v>
+        <v>13.01</v>
       </c>
       <c r="D50" s="18">
-        <v>45367</v>
+        <v>45366</v>
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
-      <c r="G50" s="39"/>
+      <c r="G50" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="15">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>208</v>
       </c>
       <c r="C51" s="29">
-        <v>18.22</v>
+        <v>10.17</v>
       </c>
       <c r="D51" s="18">
-        <v>45367</v>
+        <v>45366</v>
       </c>
       <c r="E51" s="17"/>
       <c r="F51" s="17"/>
-      <c r="G51" s="39"/>
+      <c r="G51" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>209</v>
       </c>
       <c r="C52" s="29">
-        <v>23.21</v>
+        <v>16.56</v>
       </c>
       <c r="D52" s="18">
-        <v>45368</v>
+        <v>45367</v>
       </c>
       <c r="E52" s="17"/>
       <c r="F52" s="17"/>
-      <c r="G52" s="39"/>
+      <c r="G52" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="15">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>210</v>
       </c>
       <c r="C53" s="29">
-        <v>28.28</v>
+        <v>7.56</v>
       </c>
       <c r="D53" s="18">
-        <v>45368</v>
+        <v>45367</v>
       </c>
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
-      <c r="G53" s="39"/>
+      <c r="G53" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="15">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>211</v>
       </c>
       <c r="C54" s="29">
-        <v>17.27</v>
+        <v>12.49</v>
       </c>
       <c r="D54" s="18">
-        <v>45369</v>
+        <v>45367</v>
       </c>
       <c r="E54" s="17"/>
       <c r="F54" s="17"/>
-      <c r="G54" s="39"/>
+      <c r="G54" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="15">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>212</v>
       </c>
       <c r="C55" s="29">
-        <v>11.51</v>
+        <v>7.13</v>
       </c>
       <c r="D55" s="18">
-        <v>45369</v>
+        <v>45367</v>
       </c>
       <c r="E55" s="17"/>
       <c r="F55" s="17"/>
-      <c r="G55" s="39"/>
+      <c r="G55" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="15">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>213</v>
       </c>
       <c r="C56" s="29">
-        <v>7.15</v>
+        <v>18.22</v>
       </c>
       <c r="D56" s="18">
-        <v>45369</v>
+        <v>45367</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
-      <c r="G56" s="39"/>
+      <c r="G56" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="15">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>214</v>
       </c>
       <c r="C57" s="29">
-        <v>9.02</v>
+        <v>23.21</v>
       </c>
       <c r="D57" s="18">
-        <v>45369</v>
+        <v>45368</v>
       </c>
       <c r="E57" s="17"/>
       <c r="F57" s="17"/>
-      <c r="G57" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A58" s="41"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A59" s="11" t="s">
+      <c r="G57" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+      <c r="A58" s="15">
+        <v>11</v>
+      </c>
+      <c r="B58" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="2"/>
+      <c r="C58" s="29">
+        <v>28.28</v>
+      </c>
+      <c r="D58" s="18">
+        <v>45368</v>
+      </c>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+      <c r="A59" s="15">
+        <v>12</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C59" s="29">
+        <v>17.27</v>
+      </c>
+      <c r="D59" s="18">
+        <v>45369</v>
+      </c>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C60" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G60" s="39"/>
+      <c r="A60" s="15">
+        <v>13</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C60" s="29">
+        <v>11.51</v>
+      </c>
+      <c r="D60" s="18">
+        <v>45369</v>
+      </c>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="15">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C61" s="29">
-        <v>26.05</v>
+        <v>7.15</v>
       </c>
       <c r="D61" s="18">
-        <v>45370</v>
+        <v>45369</v>
       </c>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
-      <c r="G61" s="39"/>
+      <c r="G61" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="15">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C62" s="29">
-        <v>12.51</v>
+        <v>9.02</v>
       </c>
       <c r="D62" s="18">
-        <v>45370</v>
+        <v>45369</v>
       </c>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
-      <c r="G62" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="15">
+      <c r="G62" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A63" s="46"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="48"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A64" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B64" s="12"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+      <c r="A65" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="C63" s="29">
-        <v>13.31</v>
-      </c>
-      <c r="D63" s="18">
-        <v>45370</v>
-      </c>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
-      <c r="A64" s="15">
+      <c r="D65" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="C64" s="29">
-        <v>24.56</v>
-      </c>
-      <c r="D64" s="18">
-        <v>45371</v>
-      </c>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="15">
+      <c r="E65" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="C65" s="29">
-        <v>18.08</v>
-      </c>
-      <c r="D65" s="18">
-        <v>45371</v>
-      </c>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="39"/>
+      <c r="F65" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>221</v>
       </c>
       <c r="C66" s="29">
-        <v>13.55</v>
+        <v>26.05</v>
       </c>
       <c r="D66" s="18">
-        <v>45371</v>
+        <v>45370</v>
       </c>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
-      <c r="G66" s="39"/>
+      <c r="G66" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>222</v>
       </c>
       <c r="C67" s="29">
-        <v>29.41</v>
+        <v>12.51</v>
       </c>
       <c r="D67" s="18">
-        <v>45372</v>
+        <v>45370</v>
       </c>
       <c r="E67" s="17"/>
       <c r="F67" s="17"/>
-      <c r="G67" s="39"/>
+      <c r="G67" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="15">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B68" s="16" t="s">
         <v>223</v>
       </c>
       <c r="C68" s="29">
-        <v>10.49</v>
+        <v>13.31</v>
       </c>
       <c r="D68" s="18">
-        <v>45372</v>
+        <v>45370</v>
       </c>
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
-      <c r="G68" s="39"/>
+      <c r="G68" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="15">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>224</v>
       </c>
       <c r="C69" s="29">
-        <v>16.02</v>
+        <v>24.56</v>
       </c>
       <c r="D69" s="18">
-        <v>45372</v>
+        <v>45371</v>
       </c>
       <c r="E69" s="17"/>
       <c r="F69" s="17"/>
-      <c r="G69" s="39"/>
+      <c r="G69" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>225</v>
       </c>
       <c r="C70" s="29">
-        <v>10.48</v>
+        <v>18.08</v>
       </c>
       <c r="D70" s="18">
-        <v>45373</v>
+        <v>45371</v>
       </c>
       <c r="E70" s="17"/>
       <c r="F70" s="17"/>
-      <c r="G70" s="39"/>
+      <c r="G70" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="15">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>226</v>
       </c>
       <c r="C71" s="29">
-        <v>20.49</v>
+        <v>13.55</v>
       </c>
       <c r="D71" s="18">
-        <v>45373</v>
+        <v>45371</v>
       </c>
       <c r="E71" s="17"/>
       <c r="F71" s="17"/>
-      <c r="G71" s="39"/>
+      <c r="G71" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
-      <c r="A72" s="21"/>
-      <c r="B72" s="39"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="31"/>
-      <c r="E72" s="39"/>
-      <c r="F72" s="39"/>
-      <c r="G72" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A73" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="12"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="26"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="2"/>
+      <c r="A72" s="15">
+        <v>7</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C72" s="29">
+        <v>29.41</v>
+      </c>
+      <c r="D72" s="18">
+        <v>45372</v>
+      </c>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+      <c r="A73" s="15">
+        <v>8</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="C73" s="29">
+        <v>10.49</v>
+      </c>
+      <c r="D73" s="18">
+        <v>45372</v>
+      </c>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
-      <c r="A74" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C74" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D74" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E74" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F74" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G74" s="39"/>
+      <c r="A74" s="15">
+        <v>9</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C74" s="29">
+        <v>16.02</v>
+      </c>
+      <c r="D74" s="18">
+        <v>45372</v>
+      </c>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="15">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="C75" s="44">
-        <v>5.1209375</v>
+        <v>230</v>
+      </c>
+      <c r="C75" s="29">
+        <v>10.48</v>
       </c>
       <c r="D75" s="18">
-        <v>45374</v>
-      </c>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="39"/>
+        <v>45373</v>
+      </c>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="15">
+        <v>11</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="C76" s="29">
+        <v>20.49</v>
+      </c>
+      <c r="D76" s="18">
+        <v>45373</v>
+      </c>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+      <c r="A77" s="21"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A78" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="12"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+      <c r="A79" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="C76" s="44">
-        <v>5.1209375</v>
-      </c>
-      <c r="D76" s="18">
-        <v>45375</v>
-      </c>
-      <c r="E76" s="19"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
-      <c r="A77" s="15">
+      <c r="C79" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="C77" s="44">
-        <v>5.1209375</v>
-      </c>
-      <c r="D77" s="18">
-        <v>45376</v>
-      </c>
-      <c r="E77" s="19"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
-      <c r="A78" s="15">
+      <c r="D79" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="C78" s="44">
-        <v>5.1209375</v>
-      </c>
-      <c r="D78" s="18">
-        <v>45377</v>
-      </c>
-      <c r="E78" s="19"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
-      <c r="A79" s="15">
+      <c r="E79" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="C79" s="29">
-        <v>10.13</v>
-      </c>
-      <c r="D79" s="18">
-        <v>45378</v>
-      </c>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="39"/>
+      <c r="F79" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G79" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="C80" s="29">
-        <v>9.05</v>
+        <v>232</v>
+      </c>
+      <c r="C80" s="49">
+        <v>5.1209375</v>
       </c>
       <c r="D80" s="18">
-        <v>45378</v>
-      </c>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="39"/>
+        <v>45374</v>
+      </c>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="C81" s="29">
-        <v>3.39</v>
+        <v>232</v>
+      </c>
+      <c r="C81" s="49">
+        <v>5.1209375</v>
       </c>
       <c r="D81" s="18">
-        <v>45378</v>
-      </c>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="39"/>
+        <v>45375</v>
+      </c>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="15">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="C82" s="29">
-        <v>8.27</v>
+        <v>232</v>
+      </c>
+      <c r="C82" s="49">
+        <v>5.1209375</v>
       </c>
       <c r="D82" s="18">
-        <v>45378</v>
-      </c>
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="39"/>
+        <v>45376</v>
+      </c>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="15">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B83" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="C83" s="29">
-        <v>7.21</v>
+      <c r="C83" s="49">
+        <v>5.1209375</v>
       </c>
       <c r="D83" s="18">
-        <v>45378</v>
-      </c>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="39"/>
+        <v>45377</v>
+      </c>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B84" s="16" t="s">
         <v>233</v>
       </c>
       <c r="C84" s="29">
-        <v>9.04</v>
+        <v>10.13</v>
       </c>
       <c r="D84" s="18">
         <v>45378</v>
       </c>
       <c r="E84" s="17"/>
       <c r="F84" s="17"/>
-      <c r="G84" s="39"/>
+      <c r="G84" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="15">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B85" s="16" t="s">
         <v>234</v>
       </c>
       <c r="C85" s="29">
-        <v>14.14</v>
+        <v>9.05</v>
       </c>
       <c r="D85" s="18">
         <v>45378</v>
       </c>
       <c r="E85" s="17"/>
       <c r="F85" s="17"/>
-      <c r="G85" s="39"/>
+      <c r="G85" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="15">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B86" s="16" t="s">
         <v>235</v>
       </c>
       <c r="C86" s="29">
-        <v>14.01</v>
+        <v>3.39</v>
       </c>
       <c r="D86" s="18">
-        <v>46840</v>
+        <v>45378</v>
       </c>
       <c r="E86" s="17"/>
       <c r="F86" s="17"/>
-      <c r="G86" s="39"/>
+      <c r="G86" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="15">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B87" s="16" t="s">
         <v>236</v>
       </c>
       <c r="C87" s="29">
-        <v>11.17</v>
+        <v>8.27</v>
       </c>
       <c r="D87" s="18">
-        <v>46840</v>
+        <v>45378</v>
       </c>
       <c r="E87" s="17"/>
       <c r="F87" s="17"/>
-      <c r="G87" s="39"/>
+      <c r="G87" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="15">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B88" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="C88" s="15">
-        <v>12</v>
+      <c r="C88" s="29">
+        <v>7.21</v>
       </c>
       <c r="D88" s="18">
-        <v>46840</v>
+        <v>45378</v>
       </c>
       <c r="E88" s="17"/>
       <c r="F88" s="17"/>
-      <c r="G88" s="39"/>
+      <c r="G88" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="15">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B89" s="16" t="s">
         <v>238</v>
       </c>
       <c r="C89" s="29">
-        <v>12.33</v>
+        <v>9.04</v>
       </c>
       <c r="D89" s="18">
-        <v>46840</v>
+        <v>45378</v>
       </c>
       <c r="E89" s="17"/>
       <c r="F89" s="17"/>
-      <c r="G89" s="39"/>
+      <c r="G89" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="15">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B90" s="16" t="s">
         <v>239</v>
       </c>
       <c r="C90" s="29">
-        <v>10.57</v>
+        <v>14.14</v>
       </c>
       <c r="D90" s="18">
-        <v>46840</v>
+        <v>45378</v>
       </c>
       <c r="E90" s="17"/>
       <c r="F90" s="17"/>
-      <c r="G90" s="39"/>
+      <c r="G90" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="15">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B91" s="16" t="s">
         <v>240</v>
       </c>
       <c r="C91" s="29">
-        <v>10.13</v>
+        <v>14.01</v>
       </c>
       <c r="D91" s="18">
-        <v>45380</v>
-      </c>
-      <c r="E91" s="18"/>
+        <v>46840</v>
+      </c>
+      <c r="E91" s="17"/>
       <c r="F91" s="17"/>
-      <c r="G91" s="39"/>
+      <c r="G91" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="15">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B92" s="16" t="s">
         <v>241</v>
       </c>
       <c r="C92" s="29">
-        <v>17.37</v>
+        <v>11.17</v>
       </c>
       <c r="D92" s="18">
-        <v>45380</v>
-      </c>
-      <c r="E92" s="18"/>
+        <v>46840</v>
+      </c>
+      <c r="E92" s="17"/>
       <c r="F92" s="17"/>
-      <c r="G92" s="39"/>
+      <c r="G92" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="15">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B93" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="C93" s="29">
-        <v>9.28</v>
+      <c r="C93" s="15">
+        <v>12</v>
       </c>
       <c r="D93" s="18">
-        <v>45380</v>
-      </c>
-      <c r="E93" s="18"/>
+        <v>46840</v>
+      </c>
+      <c r="E93" s="17"/>
       <c r="F93" s="17"/>
-      <c r="G93" s="39"/>
+      <c r="G93" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="15">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B94" s="16" t="s">
         <v>243</v>
       </c>
       <c r="C94" s="29">
-        <v>7.18</v>
+        <v>12.33</v>
       </c>
       <c r="D94" s="18">
-        <v>45380</v>
-      </c>
-      <c r="E94" s="18"/>
+        <v>46840</v>
+      </c>
+      <c r="E94" s="17"/>
       <c r="F94" s="17"/>
-      <c r="G94" s="39"/>
+      <c r="G94" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="15">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B95" s="16" t="s">
         <v>244</v>
       </c>
       <c r="C95" s="29">
-        <v>7.54</v>
+        <v>10.57</v>
       </c>
       <c r="D95" s="18">
-        <v>45380</v>
-      </c>
-      <c r="E95" s="18"/>
+        <v>46840</v>
+      </c>
+      <c r="E95" s="17"/>
       <c r="F95" s="17"/>
-      <c r="G95" s="39"/>
+      <c r="G95" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="15">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B96" s="16" t="s">
         <v>245</v>
       </c>
       <c r="C96" s="29">
-        <v>25.46</v>
+        <v>10.13</v>
       </c>
       <c r="D96" s="18">
-        <v>45381</v>
+        <v>45380</v>
       </c>
       <c r="E96" s="18"/>
       <c r="F96" s="17"/>
-      <c r="G96" s="39"/>
+      <c r="G96" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="15">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B97" s="16" t="s">
         <v>246</v>
       </c>
       <c r="C97" s="29">
-        <v>8.47</v>
+        <v>17.37</v>
       </c>
       <c r="D97" s="18">
-        <v>45381</v>
+        <v>45380</v>
       </c>
       <c r="E97" s="18"/>
       <c r="F97" s="17"/>
-      <c r="G97" s="39"/>
+      <c r="G97" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="15">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B98" s="16" t="s">
         <v>247</v>
       </c>
       <c r="C98" s="29">
-        <v>5.43</v>
+        <v>9.28</v>
       </c>
       <c r="D98" s="18">
-        <v>45381</v>
+        <v>45380</v>
       </c>
       <c r="E98" s="18"/>
       <c r="F98" s="17"/>
-      <c r="G98" s="39"/>
+      <c r="G98" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="15">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B99" s="16" t="s">
         <v>248</v>
       </c>
       <c r="C99" s="29">
-        <v>12.35</v>
+        <v>7.18</v>
       </c>
       <c r="D99" s="18">
-        <v>45381</v>
+        <v>45380</v>
       </c>
       <c r="E99" s="18"/>
       <c r="F99" s="17"/>
-      <c r="G99" s="39"/>
+      <c r="G99" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="15">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B100" s="16" t="s">
         <v>249</v>
       </c>
       <c r="C100" s="29">
-        <v>4.06</v>
+        <v>7.54</v>
       </c>
       <c r="D100" s="18">
-        <v>45381</v>
+        <v>45380</v>
       </c>
       <c r="E100" s="18"/>
       <c r="F100" s="17"/>
-      <c r="G100" s="39"/>
+      <c r="G100" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="15">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B101" s="16" t="s">
         <v>250</v>
       </c>
       <c r="C101" s="29">
-        <v>14.59</v>
+        <v>25.46</v>
       </c>
       <c r="D101" s="18">
-        <v>45382</v>
+        <v>45381</v>
       </c>
       <c r="E101" s="18"/>
       <c r="F101" s="17"/>
-      <c r="G101" s="39"/>
+      <c r="G101" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="15">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B102" s="16" t="s">
         <v>251</v>
       </c>
       <c r="C102" s="29">
-        <v>18.2</v>
+        <v>8.47</v>
       </c>
       <c r="D102" s="18">
-        <v>45382</v>
+        <v>45381</v>
       </c>
       <c r="E102" s="18"/>
       <c r="F102" s="17"/>
-      <c r="G102" s="39"/>
+      <c r="G102" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="15">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B103" s="16" t="s">
         <v>252</v>
       </c>
       <c r="C103" s="29">
-        <v>13.41</v>
+        <v>5.43</v>
       </c>
       <c r="D103" s="18">
-        <v>45382</v>
+        <v>45381</v>
       </c>
       <c r="E103" s="18"/>
       <c r="F103" s="17"/>
-      <c r="G103" s="39"/>
+      <c r="G103" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="15">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B104" s="16" t="s">
         <v>253</v>
       </c>
       <c r="C104" s="29">
-        <v>11.59</v>
+        <v>12.35</v>
       </c>
       <c r="D104" s="18">
-        <v>45382</v>
+        <v>45381</v>
       </c>
       <c r="E104" s="18"/>
       <c r="F104" s="17"/>
-      <c r="G104" s="39"/>
+      <c r="G104" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
-      <c r="A105" s="21"/>
-      <c r="B105" s="39"/>
-      <c r="C105" s="30"/>
-      <c r="D105" s="31"/>
-      <c r="E105" s="45"/>
-      <c r="F105" s="39"/>
-      <c r="G105" s="39"/>
+      <c r="A105" s="15">
+        <v>26</v>
+      </c>
+      <c r="B105" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C105" s="29">
+        <v>4.06</v>
+      </c>
+      <c r="D105" s="18">
+        <v>45381</v>
+      </c>
+      <c r="E105" s="18"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
-      <c r="A106" s="21"/>
-      <c r="B106" s="39"/>
-      <c r="C106" s="30"/>
-      <c r="D106" s="31"/>
-      <c r="E106" s="45"/>
-      <c r="F106" s="39"/>
-      <c r="G106" s="39"/>
+      <c r="A106" s="15">
+        <v>27</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="C106" s="29">
+        <v>14.59</v>
+      </c>
+      <c r="D106" s="18">
+        <v>45382</v>
+      </c>
+      <c r="E106" s="18"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
-      <c r="A107" s="21"/>
-      <c r="B107" s="39"/>
-      <c r="C107" s="30"/>
-      <c r="D107" s="31"/>
-      <c r="E107" s="45"/>
-      <c r="F107" s="39"/>
-      <c r="G107" s="39"/>
+      <c r="A107" s="15">
+        <v>28</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C107" s="29">
+        <v>18.2</v>
+      </c>
+      <c r="D107" s="18">
+        <v>45382</v>
+      </c>
+      <c r="E107" s="18"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
-      <c r="A108" s="21"/>
-      <c r="B108" s="39"/>
-      <c r="C108" s="30"/>
-      <c r="D108" s="31"/>
-      <c r="E108" s="45"/>
-      <c r="F108" s="39"/>
-      <c r="G108" s="39"/>
+      <c r="A108" s="15">
+        <v>29</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="C108" s="29">
+        <v>13.41</v>
+      </c>
+      <c r="D108" s="18">
+        <v>45382</v>
+      </c>
+      <c r="E108" s="18"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
-      <c r="A109" s="21"/>
-      <c r="B109" s="39"/>
-      <c r="C109" s="30"/>
-      <c r="D109" s="31"/>
-      <c r="E109" s="45"/>
-      <c r="F109" s="39"/>
-      <c r="G109" s="39"/>
+      <c r="A109" s="15">
+        <v>30</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="C109" s="29">
+        <v>11.59</v>
+      </c>
+      <c r="D109" s="18">
+        <v>45382</v>
+      </c>
+      <c r="E109" s="18"/>
+      <c r="F109" s="17"/>
+      <c r="G109" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="21"/>
-      <c r="B110" s="39"/>
+      <c r="B110" s="44"/>
       <c r="C110" s="30"/>
       <c r="D110" s="31"/>
-      <c r="E110" s="45"/>
-      <c r="F110" s="39"/>
-      <c r="G110" s="39"/>
+      <c r="E110" s="50"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="21"/>
-      <c r="B111" s="39"/>
+      <c r="B111" s="44"/>
       <c r="C111" s="30"/>
       <c r="D111" s="31"/>
-      <c r="E111" s="45"/>
-      <c r="F111" s="39"/>
-      <c r="G111" s="39"/>
+      <c r="E111" s="50"/>
+      <c r="F111" s="44"/>
+      <c r="G111" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="21"/>
-      <c r="B112" s="39"/>
+      <c r="B112" s="44"/>
       <c r="C112" s="30"/>
       <c r="D112" s="31"/>
-      <c r="E112" s="45"/>
-      <c r="F112" s="39"/>
-      <c r="G112" s="39"/>
+      <c r="E112" s="50"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="21"/>
-      <c r="B113" s="39"/>
+      <c r="B113" s="44"/>
       <c r="C113" s="30"/>
       <c r="D113" s="31"/>
-      <c r="E113" s="45"/>
-      <c r="F113" s="39"/>
-      <c r="G113" s="39"/>
+      <c r="E113" s="50"/>
+      <c r="F113" s="44"/>
+      <c r="G113" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="21"/>
-      <c r="B114" s="39"/>
+      <c r="B114" s="44"/>
       <c r="C114" s="30"/>
       <c r="D114" s="31"/>
-      <c r="E114" s="45"/>
-      <c r="F114" s="39"/>
-      <c r="G114" s="39"/>
+      <c r="E114" s="50"/>
+      <c r="F114" s="44"/>
+      <c r="G114" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="21"/>
-      <c r="B115" s="39"/>
+      <c r="B115" s="44"/>
       <c r="C115" s="30"/>
       <c r="D115" s="31"/>
-      <c r="E115" s="45"/>
-      <c r="F115" s="39"/>
-      <c r="G115" s="39"/>
+      <c r="E115" s="50"/>
+      <c r="F115" s="44"/>
+      <c r="G115" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="21"/>
-      <c r="B116" s="39"/>
+      <c r="B116" s="44"/>
       <c r="C116" s="30"/>
       <c r="D116" s="31"/>
-      <c r="E116" s="45"/>
-      <c r="F116" s="39"/>
-      <c r="G116" s="39"/>
+      <c r="E116" s="50"/>
+      <c r="F116" s="44"/>
+      <c r="G116" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="21"/>
-      <c r="B117" s="39"/>
+      <c r="B117" s="44"/>
       <c r="C117" s="30"/>
       <c r="D117" s="31"/>
-      <c r="E117" s="45"/>
-      <c r="F117" s="39"/>
-      <c r="G117" s="39"/>
+      <c r="E117" s="50"/>
+      <c r="F117" s="44"/>
+      <c r="G117" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="21"/>
-      <c r="B118" s="39"/>
+      <c r="B118" s="44"/>
       <c r="C118" s="30"/>
       <c r="D118" s="31"/>
-      <c r="E118" s="45"/>
-      <c r="F118" s="39"/>
-      <c r="G118" s="39"/>
+      <c r="E118" s="50"/>
+      <c r="F118" s="44"/>
+      <c r="G118" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="21"/>
-      <c r="B119" s="39"/>
+      <c r="B119" s="44"/>
       <c r="C119" s="30"/>
       <c r="D119" s="31"/>
-      <c r="E119" s="45"/>
-      <c r="F119" s="39"/>
-      <c r="G119" s="39"/>
+      <c r="E119" s="50"/>
+      <c r="F119" s="44"/>
+      <c r="G119" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="21"/>
-      <c r="B120" s="39"/>
+      <c r="B120" s="44"/>
       <c r="C120" s="30"/>
       <c r="D120" s="31"/>
-      <c r="E120" s="45"/>
-      <c r="F120" s="39"/>
-      <c r="G120" s="39"/>
+      <c r="E120" s="50"/>
+      <c r="F120" s="44"/>
+      <c r="G120" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="21"/>
-      <c r="B121" s="39"/>
+      <c r="B121" s="44"/>
       <c r="C121" s="30"/>
       <c r="D121" s="31"/>
-      <c r="E121" s="45"/>
-      <c r="F121" s="39"/>
-      <c r="G121" s="39"/>
+      <c r="E121" s="50"/>
+      <c r="F121" s="44"/>
+      <c r="G121" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="21"/>
-      <c r="B122" s="39"/>
+      <c r="B122" s="44"/>
       <c r="C122" s="30"/>
       <c r="D122" s="31"/>
-      <c r="E122" s="45"/>
-      <c r="F122" s="39"/>
-      <c r="G122" s="39"/>
+      <c r="E122" s="50"/>
+      <c r="F122" s="44"/>
+      <c r="G122" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="21"/>
-      <c r="B123" s="39"/>
+      <c r="B123" s="44"/>
       <c r="C123" s="30"/>
       <c r="D123" s="31"/>
-      <c r="E123" s="45"/>
-      <c r="F123" s="39"/>
-      <c r="G123" s="39"/>
+      <c r="E123" s="50"/>
+      <c r="F123" s="44"/>
+      <c r="G123" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="21"/>
-      <c r="B124" s="39"/>
+      <c r="B124" s="44"/>
       <c r="C124" s="30"/>
       <c r="D124" s="31"/>
-      <c r="E124" s="45"/>
-      <c r="F124" s="39"/>
-      <c r="G124" s="39"/>
+      <c r="E124" s="50"/>
+      <c r="F124" s="44"/>
+      <c r="G124" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="21"/>
-      <c r="B125" s="39"/>
+      <c r="B125" s="44"/>
       <c r="C125" s="30"/>
       <c r="D125" s="31"/>
-      <c r="E125" s="45"/>
-      <c r="F125" s="39"/>
-      <c r="G125" s="39"/>
+      <c r="E125" s="50"/>
+      <c r="F125" s="44"/>
+      <c r="G125" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="21"/>
-      <c r="B126" s="39"/>
+      <c r="B126" s="44"/>
       <c r="C126" s="30"/>
       <c r="D126" s="31"/>
-      <c r="E126" s="45"/>
-      <c r="F126" s="39"/>
-      <c r="G126" s="39"/>
+      <c r="E126" s="50"/>
+      <c r="F126" s="44"/>
+      <c r="G126" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="21"/>
-      <c r="B127" s="39"/>
+      <c r="B127" s="44"/>
       <c r="C127" s="30"/>
       <c r="D127" s="31"/>
-      <c r="E127" s="45"/>
-      <c r="F127" s="39"/>
-      <c r="G127" s="39"/>
+      <c r="E127" s="50"/>
+      <c r="F127" s="44"/>
+      <c r="G127" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="21"/>
-      <c r="B128" s="39"/>
+      <c r="B128" s="44"/>
       <c r="C128" s="30"/>
       <c r="D128" s="31"/>
-      <c r="E128" s="45"/>
-      <c r="F128" s="39"/>
-      <c r="G128" s="39"/>
+      <c r="E128" s="50"/>
+      <c r="F128" s="44"/>
+      <c r="G128" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="21"/>
-      <c r="B129" s="39"/>
+      <c r="B129" s="44"/>
       <c r="C129" s="30"/>
       <c r="D129" s="31"/>
-      <c r="E129" s="45"/>
-      <c r="F129" s="39"/>
-      <c r="G129" s="39"/>
+      <c r="E129" s="50"/>
+      <c r="F129" s="44"/>
+      <c r="G129" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="21"/>
-      <c r="B130" s="39"/>
+      <c r="B130" s="44"/>
       <c r="C130" s="30"/>
       <c r="D130" s="31"/>
-      <c r="E130" s="45"/>
-      <c r="F130" s="39"/>
-      <c r="G130" s="39"/>
+      <c r="E130" s="50"/>
+      <c r="F130" s="44"/>
+      <c r="G130" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="21"/>
-      <c r="B131" s="39"/>
+      <c r="B131" s="44"/>
       <c r="C131" s="30"/>
       <c r="D131" s="31"/>
-      <c r="E131" s="45"/>
-      <c r="F131" s="39"/>
-      <c r="G131" s="39"/>
+      <c r="E131" s="50"/>
+      <c r="F131" s="44"/>
+      <c r="G131" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="21"/>
-      <c r="B132" s="39"/>
+      <c r="B132" s="44"/>
       <c r="C132" s="30"/>
       <c r="D132" s="31"/>
-      <c r="E132" s="45"/>
-      <c r="F132" s="39"/>
-      <c r="G132" s="39"/>
+      <c r="E132" s="50"/>
+      <c r="F132" s="44"/>
+      <c r="G132" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="21"/>
-      <c r="B133" s="39"/>
+      <c r="B133" s="44"/>
       <c r="C133" s="30"/>
       <c r="D133" s="31"/>
-      <c r="E133" s="45"/>
-      <c r="F133" s="39"/>
-      <c r="G133" s="39"/>
+      <c r="E133" s="50"/>
+      <c r="F133" s="44"/>
+      <c r="G133" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="21"/>
-      <c r="B134" s="39"/>
+      <c r="B134" s="44"/>
       <c r="C134" s="30"/>
       <c r="D134" s="31"/>
-      <c r="E134" s="45"/>
-      <c r="F134" s="39"/>
-      <c r="G134" s="39"/>
+      <c r="E134" s="50"/>
+      <c r="F134" s="44"/>
+      <c r="G134" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
       <c r="A135" s="21"/>
-      <c r="B135" s="39"/>
+      <c r="B135" s="44"/>
       <c r="C135" s="30"/>
       <c r="D135" s="31"/>
-      <c r="E135" s="45"/>
-      <c r="F135" s="39"/>
-      <c r="G135" s="39"/>
+      <c r="E135" s="50"/>
+      <c r="F135" s="44"/>
+      <c r="G135" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="21"/>
-      <c r="B136" s="39"/>
+      <c r="B136" s="44"/>
       <c r="C136" s="30"/>
       <c r="D136" s="31"/>
-      <c r="E136" s="45"/>
-      <c r="F136" s="39"/>
-      <c r="G136" s="39"/>
+      <c r="E136" s="50"/>
+      <c r="F136" s="44"/>
+      <c r="G136" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="21"/>
-      <c r="B137" s="39"/>
+      <c r="B137" s="44"/>
       <c r="C137" s="30"/>
       <c r="D137" s="31"/>
-      <c r="E137" s="45"/>
-      <c r="F137" s="39"/>
-      <c r="G137" s="39"/>
+      <c r="E137" s="50"/>
+      <c r="F137" s="44"/>
+      <c r="G137" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
       <c r="A138" s="21"/>
-      <c r="B138" s="39"/>
+      <c r="B138" s="44"/>
       <c r="C138" s="30"/>
       <c r="D138" s="31"/>
-      <c r="E138" s="45"/>
-      <c r="F138" s="39"/>
-      <c r="G138" s="39"/>
+      <c r="E138" s="50"/>
+      <c r="F138" s="44"/>
+      <c r="G138" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
       <c r="A139" s="21"/>
-      <c r="B139" s="39"/>
+      <c r="B139" s="44"/>
       <c r="C139" s="30"/>
       <c r="D139" s="31"/>
-      <c r="E139" s="45"/>
-      <c r="F139" s="39"/>
-      <c r="G139" s="39"/>
+      <c r="E139" s="50"/>
+      <c r="F139" s="44"/>
+      <c r="G139" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="21"/>
-      <c r="B140" s="39"/>
+      <c r="B140" s="44"/>
       <c r="C140" s="30"/>
       <c r="D140" s="31"/>
-      <c r="E140" s="45"/>
-      <c r="F140" s="39"/>
-      <c r="G140" s="39"/>
+      <c r="E140" s="50"/>
+      <c r="F140" s="44"/>
+      <c r="G140" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
       <c r="A141" s="21"/>
-      <c r="B141" s="39"/>
+      <c r="B141" s="44"/>
       <c r="C141" s="30"/>
       <c r="D141" s="31"/>
-      <c r="E141" s="45"/>
-      <c r="F141" s="39"/>
-      <c r="G141" s="39"/>
+      <c r="E141" s="50"/>
+      <c r="F141" s="44"/>
+      <c r="G141" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
       <c r="A142" s="21"/>
-      <c r="B142" s="39"/>
+      <c r="B142" s="44"/>
       <c r="C142" s="30"/>
       <c r="D142" s="31"/>
-      <c r="E142" s="45"/>
-      <c r="F142" s="39"/>
-      <c r="G142" s="39"/>
+      <c r="E142" s="50"/>
+      <c r="F142" s="44"/>
+      <c r="G142" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="21"/>
-      <c r="B143" s="39"/>
+      <c r="B143" s="44"/>
       <c r="C143" s="30"/>
       <c r="D143" s="31"/>
-      <c r="E143" s="45"/>
-      <c r="F143" s="39"/>
-      <c r="G143" s="39"/>
+      <c r="E143" s="50"/>
+      <c r="F143" s="44"/>
+      <c r="G143" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
       <c r="A144" s="21"/>
-      <c r="B144" s="39"/>
+      <c r="B144" s="44"/>
       <c r="C144" s="30"/>
       <c r="D144" s="31"/>
-      <c r="E144" s="45"/>
-      <c r="F144" s="39"/>
-      <c r="G144" s="39"/>
+      <c r="E144" s="50"/>
+      <c r="F144" s="44"/>
+      <c r="G144" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="21"/>
-      <c r="B145" s="39"/>
+      <c r="B145" s="44"/>
       <c r="C145" s="30"/>
       <c r="D145" s="31"/>
-      <c r="E145" s="45"/>
-      <c r="F145" s="39"/>
-      <c r="G145" s="39"/>
+      <c r="E145" s="50"/>
+      <c r="F145" s="44"/>
+      <c r="G145" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="21"/>
-      <c r="B146" s="39"/>
+      <c r="B146" s="44"/>
       <c r="C146" s="30"/>
       <c r="D146" s="31"/>
-      <c r="E146" s="45"/>
-      <c r="F146" s="39"/>
-      <c r="G146" s="39"/>
+      <c r="E146" s="50"/>
+      <c r="F146" s="44"/>
+      <c r="G146" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="21"/>
-      <c r="B147" s="39"/>
+      <c r="B147" s="44"/>
       <c r="C147" s="30"/>
       <c r="D147" s="31"/>
-      <c r="E147" s="45"/>
-      <c r="F147" s="39"/>
-      <c r="G147" s="39"/>
+      <c r="E147" s="50"/>
+      <c r="F147" s="44"/>
+      <c r="G147" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="21"/>
-      <c r="B148" s="39"/>
+      <c r="B148" s="44"/>
       <c r="C148" s="30"/>
       <c r="D148" s="31"/>
-      <c r="E148" s="45"/>
-      <c r="F148" s="39"/>
-      <c r="G148" s="39"/>
+      <c r="E148" s="50"/>
+      <c r="F148" s="44"/>
+      <c r="G148" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="21"/>
-      <c r="B149" s="39"/>
+      <c r="B149" s="44"/>
       <c r="C149" s="30"/>
       <c r="D149" s="31"/>
-      <c r="E149" s="45"/>
-      <c r="F149" s="39"/>
-      <c r="G149" s="39"/>
+      <c r="E149" s="50"/>
+      <c r="F149" s="44"/>
+      <c r="G149" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
       <c r="A150" s="21"/>
-      <c r="B150" s="39"/>
+      <c r="B150" s="44"/>
       <c r="C150" s="30"/>
       <c r="D150" s="31"/>
-      <c r="E150" s="45"/>
-      <c r="F150" s="39"/>
-      <c r="G150" s="39"/>
+      <c r="E150" s="50"/>
+      <c r="F150" s="44"/>
+      <c r="G150" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="21"/>
-      <c r="B151" s="39"/>
+      <c r="B151" s="44"/>
       <c r="C151" s="30"/>
       <c r="D151" s="31"/>
-      <c r="E151" s="45"/>
-      <c r="F151" s="39"/>
-      <c r="G151" s="39"/>
+      <c r="E151" s="50"/>
+      <c r="F151" s="44"/>
+      <c r="G151" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="21"/>
-      <c r="B152" s="39"/>
+      <c r="B152" s="44"/>
       <c r="C152" s="30"/>
       <c r="D152" s="31"/>
-      <c r="E152" s="45"/>
-      <c r="F152" s="39"/>
-      <c r="G152" s="39"/>
+      <c r="E152" s="50"/>
+      <c r="F152" s="44"/>
+      <c r="G152" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="21"/>
-      <c r="B153" s="39"/>
+      <c r="B153" s="44"/>
       <c r="C153" s="30"/>
       <c r="D153" s="31"/>
-      <c r="E153" s="45"/>
-      <c r="F153" s="39"/>
-      <c r="G153" s="39"/>
+      <c r="E153" s="50"/>
+      <c r="F153" s="44"/>
+      <c r="G153" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="21"/>
-      <c r="B154" s="39"/>
+      <c r="B154" s="44"/>
       <c r="C154" s="30"/>
       <c r="D154" s="31"/>
-      <c r="E154" s="45"/>
-      <c r="F154" s="39"/>
-      <c r="G154" s="39"/>
+      <c r="E154" s="50"/>
+      <c r="F154" s="44"/>
+      <c r="G154" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="21"/>
-      <c r="B155" s="39"/>
+      <c r="B155" s="44"/>
       <c r="C155" s="30"/>
       <c r="D155" s="31"/>
-      <c r="E155" s="45"/>
-      <c r="F155" s="39"/>
-      <c r="G155" s="39"/>
+      <c r="E155" s="50"/>
+      <c r="F155" s="44"/>
+      <c r="G155" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="21"/>
-      <c r="B156" s="39"/>
+      <c r="B156" s="44"/>
       <c r="C156" s="30"/>
       <c r="D156" s="31"/>
-      <c r="E156" s="45"/>
-      <c r="F156" s="39"/>
-      <c r="G156" s="39"/>
+      <c r="E156" s="50"/>
+      <c r="F156" s="44"/>
+      <c r="G156" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="21"/>
-      <c r="B157" s="39"/>
+      <c r="B157" s="44"/>
       <c r="C157" s="30"/>
       <c r="D157" s="31"/>
-      <c r="E157" s="45"/>
-      <c r="F157" s="39"/>
-      <c r="G157" s="39"/>
+      <c r="E157" s="50"/>
+      <c r="F157" s="44"/>
+      <c r="G157" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="21"/>
-      <c r="B158" s="39"/>
+      <c r="B158" s="44"/>
       <c r="C158" s="30"/>
       <c r="D158" s="31"/>
-      <c r="E158" s="45"/>
-      <c r="F158" s="39"/>
-      <c r="G158" s="39"/>
+      <c r="E158" s="50"/>
+      <c r="F158" s="44"/>
+      <c r="G158" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="21"/>
-      <c r="B159" s="39"/>
+      <c r="B159" s="44"/>
       <c r="C159" s="30"/>
       <c r="D159" s="31"/>
-      <c r="E159" s="45"/>
-      <c r="F159" s="39"/>
-      <c r="G159" s="39"/>
+      <c r="E159" s="50"/>
+      <c r="F159" s="44"/>
+      <c r="G159" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="21"/>
-      <c r="B160" s="39"/>
+      <c r="B160" s="44"/>
       <c r="C160" s="30"/>
       <c r="D160" s="31"/>
-      <c r="E160" s="45"/>
-      <c r="F160" s="39"/>
-      <c r="G160" s="39"/>
+      <c r="E160" s="50"/>
+      <c r="F160" s="44"/>
+      <c r="G160" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="21"/>
-      <c r="B161" s="39"/>
+      <c r="B161" s="44"/>
       <c r="C161" s="30"/>
       <c r="D161" s="31"/>
-      <c r="E161" s="45"/>
-      <c r="F161" s="39"/>
-      <c r="G161" s="39"/>
+      <c r="E161" s="50"/>
+      <c r="F161" s="44"/>
+      <c r="G161" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="21"/>
-      <c r="B162" s="39"/>
+      <c r="B162" s="44"/>
       <c r="C162" s="30"/>
       <c r="D162" s="31"/>
-      <c r="E162" s="45"/>
-      <c r="F162" s="39"/>
-      <c r="G162" s="39"/>
+      <c r="E162" s="50"/>
+      <c r="F162" s="44"/>
+      <c r="G162" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="21"/>
-      <c r="B163" s="39"/>
+      <c r="B163" s="44"/>
       <c r="C163" s="30"/>
       <c r="D163" s="31"/>
-      <c r="E163" s="45"/>
-      <c r="F163" s="39"/>
-      <c r="G163" s="39"/>
+      <c r="E163" s="50"/>
+      <c r="F163" s="44"/>
+      <c r="G163" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="21"/>
-      <c r="B164" s="39"/>
+      <c r="B164" s="44"/>
       <c r="C164" s="30"/>
       <c r="D164" s="31"/>
-      <c r="E164" s="45"/>
-      <c r="F164" s="39"/>
-      <c r="G164" s="39"/>
+      <c r="E164" s="50"/>
+      <c r="F164" s="44"/>
+      <c r="G164" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="21"/>
-      <c r="B165" s="39"/>
+      <c r="B165" s="44"/>
       <c r="C165" s="30"/>
       <c r="D165" s="31"/>
-      <c r="E165" s="45"/>
-      <c r="F165" s="39"/>
-      <c r="G165" s="39"/>
+      <c r="E165" s="50"/>
+      <c r="F165" s="44"/>
+      <c r="G165" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
       <c r="A166" s="21"/>
-      <c r="B166" s="39"/>
+      <c r="B166" s="44"/>
       <c r="C166" s="30"/>
       <c r="D166" s="31"/>
-      <c r="E166" s="45"/>
-      <c r="F166" s="39"/>
-      <c r="G166" s="39"/>
+      <c r="E166" s="50"/>
+      <c r="F166" s="44"/>
+      <c r="G166" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="21"/>
-      <c r="B167" s="39"/>
+      <c r="B167" s="44"/>
       <c r="C167" s="30"/>
       <c r="D167" s="31"/>
-      <c r="E167" s="45"/>
-      <c r="F167" s="39"/>
-      <c r="G167" s="39"/>
+      <c r="E167" s="50"/>
+      <c r="F167" s="44"/>
+      <c r="G167" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
       <c r="A168" s="21"/>
-      <c r="B168" s="39"/>
+      <c r="B168" s="44"/>
       <c r="C168" s="30"/>
       <c r="D168" s="31"/>
-      <c r="E168" s="45"/>
-      <c r="F168" s="39"/>
-      <c r="G168" s="39"/>
+      <c r="E168" s="50"/>
+      <c r="F168" s="44"/>
+      <c r="G168" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
       <c r="A169" s="21"/>
-      <c r="B169" s="39"/>
+      <c r="B169" s="44"/>
       <c r="C169" s="30"/>
       <c r="D169" s="31"/>
-      <c r="E169" s="45"/>
-      <c r="F169" s="39"/>
-      <c r="G169" s="39"/>
+      <c r="E169" s="50"/>
+      <c r="F169" s="44"/>
+      <c r="G169" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
       <c r="A170" s="21"/>
-      <c r="B170" s="39"/>
+      <c r="B170" s="44"/>
       <c r="C170" s="30"/>
       <c r="D170" s="31"/>
-      <c r="E170" s="45"/>
-      <c r="F170" s="39"/>
-      <c r="G170" s="39"/>
+      <c r="E170" s="50"/>
+      <c r="F170" s="44"/>
+      <c r="G170" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="21"/>
-      <c r="B171" s="2"/>
-      <c r="C171" s="46"/>
+      <c r="B171" s="44"/>
+      <c r="C171" s="30"/>
       <c r="D171" s="31"/>
-      <c r="E171" s="39"/>
-      <c r="F171" s="39"/>
-      <c r="G171" s="39"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A172" s="41"/>
-      <c r="B172" s="2"/>
-      <c r="C172" s="42"/>
-      <c r="D172" s="43"/>
-      <c r="E172" s="2"/>
-      <c r="F172" s="2"/>
-      <c r="G172" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A173" s="41"/>
-      <c r="B173" s="2"/>
-      <c r="C173" s="42"/>
-      <c r="D173" s="43"/>
-      <c r="E173" s="2"/>
-      <c r="F173" s="2"/>
-      <c r="G173" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A174" s="41"/>
-      <c r="B174" s="2"/>
-      <c r="C174" s="42"/>
-      <c r="D174" s="43"/>
-      <c r="E174" s="2"/>
-      <c r="F174" s="2"/>
-      <c r="G174" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A175" s="41"/>
-      <c r="B175" s="2"/>
-      <c r="C175" s="42"/>
-      <c r="D175" s="43"/>
-      <c r="E175" s="2"/>
-      <c r="F175" s="2"/>
-      <c r="G175" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A176" s="41"/>
+      <c r="E171" s="50"/>
+      <c r="F171" s="44"/>
+      <c r="G171" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
+      <c r="A172" s="21"/>
+      <c r="B172" s="44"/>
+      <c r="C172" s="30"/>
+      <c r="D172" s="31"/>
+      <c r="E172" s="50"/>
+      <c r="F172" s="44"/>
+      <c r="G172" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
+      <c r="A173" s="21"/>
+      <c r="B173" s="44"/>
+      <c r="C173" s="30"/>
+      <c r="D173" s="31"/>
+      <c r="E173" s="50"/>
+      <c r="F173" s="44"/>
+      <c r="G173" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
+      <c r="A174" s="21"/>
+      <c r="B174" s="44"/>
+      <c r="C174" s="30"/>
+      <c r="D174" s="31"/>
+      <c r="E174" s="50"/>
+      <c r="F174" s="44"/>
+      <c r="G174" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
+      <c r="A175" s="21"/>
+      <c r="B175" s="44"/>
+      <c r="C175" s="30"/>
+      <c r="D175" s="31"/>
+      <c r="E175" s="50"/>
+      <c r="F175" s="44"/>
+      <c r="G175" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
+      <c r="A176" s="21"/>
       <c r="B176" s="2"/>
-      <c r="C176" s="42"/>
-      <c r="D176" s="43"/>
-      <c r="E176" s="2"/>
-      <c r="F176" s="2"/>
-      <c r="G176" s="2"/>
+      <c r="C176" s="51"/>
+      <c r="D176" s="31"/>
+      <c r="E176" s="44"/>
+      <c r="F176" s="44"/>
+      <c r="G176" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A177" s="41"/>
+      <c r="A177" s="46"/>
       <c r="B177" s="2"/>
-      <c r="C177" s="42"/>
-      <c r="D177" s="43"/>
+      <c r="C177" s="47"/>
+      <c r="D177" s="48"/>
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
       <c r="G177" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A178" s="41"/>
+      <c r="A178" s="46"/>
       <c r="B178" s="2"/>
-      <c r="C178" s="42"/>
-      <c r="D178" s="43"/>
+      <c r="C178" s="47"/>
+      <c r="D178" s="48"/>
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A179" s="41"/>
+      <c r="A179" s="46"/>
       <c r="B179" s="2"/>
-      <c r="C179" s="42"/>
-      <c r="D179" s="43"/>
+      <c r="C179" s="47"/>
+      <c r="D179" s="48"/>
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
       <c r="G179" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A180" s="41"/>
+      <c r="A180" s="46"/>
       <c r="B180" s="2"/>
-      <c r="C180" s="42"/>
-      <c r="D180" s="43"/>
+      <c r="C180" s="47"/>
+      <c r="D180" s="48"/>
       <c r="E180" s="2"/>
       <c r="F180" s="2"/>
       <c r="G180" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A181" s="41"/>
+      <c r="A181" s="46"/>
       <c r="B181" s="2"/>
-      <c r="C181" s="42"/>
-      <c r="D181" s="43"/>
+      <c r="C181" s="47"/>
+      <c r="D181" s="48"/>
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
       <c r="G181" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A182" s="41"/>
+      <c r="A182" s="46"/>
       <c r="B182" s="2"/>
-      <c r="C182" s="42"/>
-      <c r="D182" s="43"/>
+      <c r="C182" s="47"/>
+      <c r="D182" s="48"/>
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
       <c r="G182" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A183" s="41"/>
+      <c r="A183" s="46"/>
       <c r="B183" s="2"/>
-      <c r="C183" s="42"/>
-      <c r="D183" s="43"/>
+      <c r="C183" s="47"/>
+      <c r="D183" s="48"/>
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
       <c r="G183" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A184" s="41"/>
+      <c r="A184" s="46"/>
       <c r="B184" s="2"/>
-      <c r="C184" s="42"/>
-      <c r="D184" s="43"/>
+      <c r="C184" s="47"/>
+      <c r="D184" s="48"/>
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A185" s="41"/>
+      <c r="A185" s="46"/>
       <c r="B185" s="2"/>
-      <c r="C185" s="42"/>
-      <c r="D185" s="43"/>
+      <c r="C185" s="47"/>
+      <c r="D185" s="48"/>
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A186" s="41"/>
+      <c r="A186" s="46"/>
       <c r="B186" s="2"/>
-      <c r="C186" s="42"/>
-      <c r="D186" s="43"/>
+      <c r="C186" s="47"/>
+      <c r="D186" s="48"/>
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A187" s="41"/>
+      <c r="A187" s="46"/>
       <c r="B187" s="2"/>
-      <c r="C187" s="42"/>
-      <c r="D187" s="43"/>
+      <c r="C187" s="47"/>
+      <c r="D187" s="48"/>
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A188" s="41"/>
+      <c r="A188" s="46"/>
       <c r="B188" s="2"/>
-      <c r="C188" s="42"/>
-      <c r="D188" s="43"/>
+      <c r="C188" s="47"/>
+      <c r="D188" s="48"/>
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A189" s="41"/>
+      <c r="A189" s="46"/>
       <c r="B189" s="2"/>
-      <c r="C189" s="42"/>
-      <c r="D189" s="43"/>
+      <c r="C189" s="47"/>
+      <c r="D189" s="48"/>
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
       <c r="G189" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A190" s="41"/>
+      <c r="A190" s="46"/>
       <c r="B190" s="2"/>
-      <c r="C190" s="42"/>
-      <c r="D190" s="43"/>
+      <c r="C190" s="47"/>
+      <c r="D190" s="48"/>
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
       <c r="G190" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A191" s="41"/>
+      <c r="A191" s="46"/>
       <c r="B191" s="2"/>
-      <c r="C191" s="42"/>
-      <c r="D191" s="43"/>
+      <c r="C191" s="47"/>
+      <c r="D191" s="48"/>
       <c r="E191" s="2"/>
       <c r="F191" s="2"/>
       <c r="G191" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A192" s="41"/>
+      <c r="A192" s="46"/>
       <c r="B192" s="2"/>
-      <c r="C192" s="42"/>
-      <c r="D192" s="43"/>
+      <c r="C192" s="47"/>
+      <c r="D192" s="48"/>
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
       <c r="G192" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A193" s="41"/>
+      <c r="A193" s="46"/>
       <c r="B193" s="2"/>
-      <c r="C193" s="42"/>
-      <c r="D193" s="43"/>
+      <c r="C193" s="47"/>
+      <c r="D193" s="48"/>
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A194" s="41"/>
+      <c r="A194" s="46"/>
       <c r="B194" s="2"/>
-      <c r="C194" s="42"/>
-      <c r="D194" s="43"/>
+      <c r="C194" s="47"/>
+      <c r="D194" s="48"/>
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A195" s="41"/>
+      <c r="A195" s="46"/>
       <c r="B195" s="2"/>
-      <c r="C195" s="42"/>
-      <c r="D195" s="43"/>
+      <c r="C195" s="47"/>
+      <c r="D195" s="48"/>
       <c r="E195" s="2"/>
       <c r="F195" s="2"/>
       <c r="G195" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A196" s="41"/>
+      <c r="A196" s="46"/>
       <c r="B196" s="2"/>
-      <c r="C196" s="42"/>
-      <c r="D196" s="43"/>
+      <c r="C196" s="47"/>
+      <c r="D196" s="48"/>
       <c r="E196" s="2"/>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A197" s="41"/>
+      <c r="A197" s="46"/>
       <c r="B197" s="2"/>
-      <c r="C197" s="42"/>
-      <c r="D197" s="43"/>
+      <c r="C197" s="47"/>
+      <c r="D197" s="48"/>
       <c r="E197" s="2"/>
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A198" s="41"/>
+      <c r="A198" s="46"/>
       <c r="B198" s="2"/>
-      <c r="C198" s="42"/>
-      <c r="D198" s="43"/>
+      <c r="C198" s="47"/>
+      <c r="D198" s="48"/>
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
       <c r="G198" s="2"/>
     </row>
+    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A199" s="46"/>
+      <c r="B199" s="2"/>
+      <c r="C199" s="47"/>
+      <c r="D199" s="48"/>
+      <c r="E199" s="2"/>
+      <c r="F199" s="2"/>
+      <c r="G199" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A200" s="46"/>
+      <c r="B200" s="2"/>
+      <c r="C200" s="47"/>
+      <c r="D200" s="48"/>
+      <c r="E200" s="2"/>
+      <c r="F200" s="2"/>
+      <c r="G200" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A201" s="46"/>
+      <c r="B201" s="2"/>
+      <c r="C201" s="47"/>
+      <c r="D201" s="48"/>
+      <c r="E201" s="2"/>
+      <c r="F201" s="2"/>
+      <c r="G201" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A202" s="46"/>
+      <c r="B202" s="2"/>
+      <c r="C202" s="47"/>
+      <c r="D202" s="48"/>
+      <c r="E202" s="2"/>
+      <c r="F202" s="2"/>
+      <c r="G202" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A203" s="46"/>
+      <c r="B203" s="2"/>
+      <c r="C203" s="47"/>
+      <c r="D203" s="48"/>
+      <c r="E203" s="2"/>
+      <c r="F203" s="2"/>
+      <c r="G203" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A78:F78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added certification details in effort tracker
</commit_message>
<xml_diff>
--- a/001EffortTracker/KT Plan.xlsx
+++ b/001EffortTracker/KT Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Index"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="291">
   <si>
     <t>Playwright: Web Automation Testing From Zero to Hero - Artem Bondar</t>
   </si>
@@ -883,7 +883,21 @@
     <t>Azure Basics</t>
   </si>
   <si>
-    <t/>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>CI/CD Pipelines</t>
+  </si>
+  <si>
+    <t>Microsoft Playwright certification Exams</t>
+  </si>
+  <si>
+    <t>Lambdatest
+V Skills</t>
+  </si>
+  <si>
+    <t>https://www.lambdatest.com/certifications/playwright-101
+https://www.vskills.in/certification/playwright-certification-course</t>
   </si>
 </sst>
 </file>
@@ -943,15 +957,15 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1003,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="54">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1107,16 +1121,7 @@
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
@@ -1130,9 +1135,6 @@
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1158,20 +1160,20 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1478,31 +1480,31 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="57" width="6.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="51" width="38.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="24" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="51" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="51" width="41.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="53" width="6.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="47" width="38.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="23" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="47" width="23.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="47" width="41.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="21"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="22"/>
@@ -1514,7 +1516,7 @@
       <c r="E2" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="48" t="s">
         <v>259</v>
       </c>
       <c r="G2" s="14" t="s">
@@ -1534,7 +1536,7 @@
       <c r="E3" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="F3" s="52">
+      <c r="F3" s="21">
         <v>1</v>
       </c>
       <c r="G3" s="17" t="s">
@@ -1552,7 +1554,7 @@
       <c r="E4" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="21">
         <v>1</v>
       </c>
       <c r="G4" s="17" t="s">
@@ -1570,7 +1572,7 @@
       <c r="E5" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="21">
         <v>1</v>
       </c>
       <c r="G5" s="17" t="s">
@@ -1588,7 +1590,7 @@
       <c r="E6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="21">
         <v>1</v>
       </c>
       <c r="G6" s="17" t="s">
@@ -1606,13 +1608,13 @@
       <c r="E7" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="21">
         <v>1</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="49" t="s">
         <v>267</v>
       </c>
     </row>
@@ -1626,7 +1628,7 @@
       <c r="E8" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="21">
         <v>2</v>
       </c>
       <c r="G8" s="17" t="s">
@@ -1644,7 +1646,7 @@
       <c r="E9" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="21">
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
@@ -1662,7 +1664,7 @@
       <c r="E10" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="21">
         <v>3</v>
       </c>
       <c r="G10" s="17" t="s">
@@ -1680,7 +1682,7 @@
       <c r="E11" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="F11" s="52">
+      <c r="F11" s="21">
         <v>3</v>
       </c>
       <c r="G11" s="17" t="s">
@@ -1698,7 +1700,7 @@
       <c r="E12" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="21">
         <v>1</v>
       </c>
       <c r="G12" s="17" t="s">
@@ -1716,7 +1718,7 @@
       <c r="E13" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F13" s="21">
         <v>3</v>
       </c>
       <c r="G13" s="17" t="s">
@@ -1734,7 +1736,7 @@
       <c r="E14" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="21">
         <v>2</v>
       </c>
       <c r="G14" s="17" t="s">
@@ -1752,13 +1754,13 @@
       <c r="E15" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F15" s="21">
         <v>3</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="H15" s="53" t="s">
+      <c r="H15" s="49" t="s">
         <v>278</v>
       </c>
     </row>
@@ -1772,13 +1774,13 @@
       <c r="E16" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F16" s="21">
         <v>1</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="H16" s="53" t="s">
+      <c r="H16" s="49" t="s">
         <v>280</v>
       </c>
     </row>
@@ -1792,13 +1794,13 @@
       <c r="E17" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="F17" s="52">
+      <c r="F17" s="21">
         <v>3</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="H17" s="53" t="s">
+      <c r="H17" s="49" t="s">
         <v>282</v>
       </c>
     </row>
@@ -1812,7 +1814,7 @@
       <c r="E18" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F18" s="21">
         <v>3</v>
       </c>
       <c r="G18" s="17" t="s">
@@ -1830,63 +1832,117 @@
       <c r="E19" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="F19" s="52">
+      <c r="F19" s="21">
         <v>1</v>
       </c>
-      <c r="G19" s="54" t="s">
+      <c r="G19" s="35" t="s">
         <v>265</v>
       </c>
-      <c r="H19" s="54"/>
+      <c r="H19" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
-      <c r="D20" s="55">
+      <c r="D20" s="48">
         <v>18</v>
       </c>
-      <c r="E20" s="54" t="s">
+      <c r="E20" s="35" t="s">
         <v>285</v>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="21">
         <v>2</v>
       </c>
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="35" t="s">
         <v>265</v>
       </c>
-      <c r="H20" s="54"/>
+      <c r="H20" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
+      <c r="D21" s="48">
+        <v>19</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="F21" s="21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="H21" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="D22" s="48">
+        <v>20</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="F22" s="21">
+        <v>1</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="H22" s="35"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="57">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="56" t="s">
-        <v>286</v>
-      </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="D23" s="50">
+        <v>21</v>
+      </c>
+      <c r="E23" s="51" t="s">
+        <v>288</v>
+      </c>
+      <c r="F23" s="52">
+        <v>1</v>
+      </c>
+      <c r="G23" s="51" t="s">
+        <v>289</v>
+      </c>
+      <c r="H23" s="51" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1900,88 +1956,88 @@
   </sheetPr>
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="23" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="51" width="60.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="47" width="60.29071428571429" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="33" width="8.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="34" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="51" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="51" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="51" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="47" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="47" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="47" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="35"/>
-      <c r="B1" s="36" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="21"/>
+      <c r="B1" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5">
-      <c r="A2" s="35">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="35">
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5">
-      <c r="A4" s="35">
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="21"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="43"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="13" t="s">
@@ -2002,7 +2058,7 @@
       <c r="F7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="43"/>
+      <c r="G7" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33">
       <c r="A8" s="15">
@@ -2021,7 +2077,7 @@
         <v>165</v>
       </c>
       <c r="F8" s="17"/>
-      <c r="G8" s="43"/>
+      <c r="G8" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="15">
@@ -2040,7 +2096,7 @@
         <v>165</v>
       </c>
       <c r="F9" s="17"/>
-      <c r="G9" s="43"/>
+      <c r="G9" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="15">
@@ -2059,7 +2115,7 @@
         <v>165</v>
       </c>
       <c r="F10" s="17"/>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="40" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2080,7 +2136,7 @@
         <v>165</v>
       </c>
       <c r="F11" s="17"/>
-      <c r="G11" s="43"/>
+      <c r="G11" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="15">
@@ -2099,7 +2155,7 @@
         <v>165</v>
       </c>
       <c r="F12" s="17"/>
-      <c r="G12" s="43"/>
+      <c r="G12" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="15">
@@ -2118,7 +2174,7 @@
         <v>165</v>
       </c>
       <c r="F13" s="17"/>
-      <c r="G13" s="43"/>
+      <c r="G13" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="15">
@@ -2137,7 +2193,7 @@
         <v>165</v>
       </c>
       <c r="F14" s="17"/>
-      <c r="G14" s="43"/>
+      <c r="G14" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="15">
@@ -2156,7 +2212,7 @@
         <v>165</v>
       </c>
       <c r="F15" s="17"/>
-      <c r="G15" s="43"/>
+      <c r="G15" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="15">
@@ -2175,7 +2231,7 @@
         <v>165</v>
       </c>
       <c r="F16" s="17"/>
-      <c r="G16" s="43"/>
+      <c r="G16" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="15">
@@ -2192,7 +2248,7 @@
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="43"/>
+      <c r="G17" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="15">
@@ -2209,7 +2265,7 @@
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
-      <c r="G18" s="43"/>
+      <c r="G18" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="15">
@@ -2226,7 +2282,7 @@
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
-      <c r="G19" s="43"/>
+      <c r="G19" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="33">
       <c r="A20" s="15">
@@ -2243,7 +2299,7 @@
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="43"/>
+      <c r="G20" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="15">
@@ -2260,7 +2316,7 @@
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
-      <c r="G21" s="43"/>
+      <c r="G21" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="15">
@@ -2277,7 +2333,7 @@
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
-      <c r="G22" s="43"/>
+      <c r="G22" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="15">
@@ -2294,7 +2350,7 @@
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
-      <c r="G23" s="43"/>
+      <c r="G23" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="15">
@@ -2311,7 +2367,7 @@
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="43"/>
+      <c r="G24" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="15">
@@ -2328,7 +2384,7 @@
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
-      <c r="G25" s="43"/>
+      <c r="G25" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="15">
@@ -2345,7 +2401,7 @@
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="43"/>
+      <c r="G26" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="33">
       <c r="A27" s="15">
@@ -2362,7 +2418,7 @@
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
-      <c r="G27" s="43"/>
+      <c r="G27" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="15">
@@ -2379,7 +2435,7 @@
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
-      <c r="G28" s="43"/>
+      <c r="G28" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="15">
@@ -2396,7 +2452,7 @@
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
-      <c r="G29" s="43"/>
+      <c r="G29" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="15">
@@ -2413,7 +2469,7 @@
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
-      <c r="G30" s="43"/>
+      <c r="G30" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="15">
@@ -2430,7 +2486,7 @@
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
-      <c r="G31" s="43"/>
+      <c r="G31" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="15">
@@ -2447,7 +2503,7 @@
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
-      <c r="G32" s="43"/>
+      <c r="G32" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="15">
@@ -2464,7 +2520,7 @@
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
-      <c r="G33" s="43"/>
+      <c r="G33" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="15">
@@ -2481,7 +2537,7 @@
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
-      <c r="G34" s="43"/>
+      <c r="G34" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="15">
@@ -2498,7 +2554,7 @@
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
-      <c r="G35" s="43"/>
+      <c r="G35" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="15">
@@ -2515,7 +2571,7 @@
       </c>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
-      <c r="G36" s="43"/>
+      <c r="G36" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="15">
@@ -2532,7 +2588,7 @@
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
-      <c r="G37" s="43"/>
+      <c r="G37" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="15">
@@ -2549,7 +2605,7 @@
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
-      <c r="G38" s="43"/>
+      <c r="G38" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="15">
@@ -2566,7 +2622,7 @@
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
-      <c r="G39" s="43"/>
+      <c r="G39" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="15">
@@ -2583,7 +2639,7 @@
       </c>
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
-      <c r="G40" s="43"/>
+      <c r="G40" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="15">
@@ -2600,7 +2656,7 @@
       </c>
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
-      <c r="G41" s="43"/>
+      <c r="G41" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="15">
@@ -2617,7 +2673,7 @@
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
-      <c r="G42" s="43"/>
+      <c r="G42" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="15">
@@ -2634,7 +2690,7 @@
       </c>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
-      <c r="G43" s="43"/>
+      <c r="G43" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="15">
@@ -2651,16 +2707,16 @@
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
-      <c r="G44" s="43"/>
+      <c r="G44" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="21"/>
-      <c r="B45" s="43"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="30"/>
       <c r="D45" s="31"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A46" s="11" t="s">
@@ -2692,7 +2748,7 @@
       <c r="F47" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="43"/>
+      <c r="G47" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="15">
@@ -2709,7 +2765,7 @@
       </c>
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
-      <c r="G48" s="43"/>
+      <c r="G48" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="15">
@@ -2726,7 +2782,7 @@
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="17"/>
-      <c r="G49" s="43"/>
+      <c r="G49" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="15">
@@ -2743,7 +2799,7 @@
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
-      <c r="G50" s="43"/>
+      <c r="G50" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="15">
@@ -2760,7 +2816,7 @@
       </c>
       <c r="E51" s="17"/>
       <c r="F51" s="17"/>
-      <c r="G51" s="43"/>
+      <c r="G51" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="15">
@@ -2777,7 +2833,7 @@
       </c>
       <c r="E52" s="17"/>
       <c r="F52" s="17"/>
-      <c r="G52" s="43"/>
+      <c r="G52" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="15">
@@ -2794,7 +2850,7 @@
       </c>
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
-      <c r="G53" s="43"/>
+      <c r="G53" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="15">
@@ -2811,7 +2867,7 @@
       </c>
       <c r="E54" s="17"/>
       <c r="F54" s="17"/>
-      <c r="G54" s="43"/>
+      <c r="G54" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="15">
@@ -2828,7 +2884,7 @@
       </c>
       <c r="E55" s="17"/>
       <c r="F55" s="17"/>
-      <c r="G55" s="43"/>
+      <c r="G55" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="15">
@@ -2845,7 +2901,7 @@
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
-      <c r="G56" s="43"/>
+      <c r="G56" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="15">
@@ -2862,7 +2918,7 @@
       </c>
       <c r="E57" s="17"/>
       <c r="F57" s="17"/>
-      <c r="G57" s="43"/>
+      <c r="G57" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="15">
@@ -2879,7 +2935,7 @@
       </c>
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
-      <c r="G58" s="43"/>
+      <c r="G58" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="15">
@@ -2896,7 +2952,7 @@
       </c>
       <c r="E59" s="17"/>
       <c r="F59" s="17"/>
-      <c r="G59" s="43"/>
+      <c r="G59" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="15">
@@ -2913,7 +2969,7 @@
       </c>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
-      <c r="G60" s="43"/>
+      <c r="G60" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="15">
@@ -2930,7 +2986,7 @@
       </c>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
-      <c r="G61" s="43"/>
+      <c r="G61" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="15">
@@ -2947,13 +3003,13 @@
       </c>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
-      <c r="G62" s="43"/>
+      <c r="G62" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A63" s="45"/>
+      <c r="A63" s="41"/>
       <c r="B63" s="2"/>
-      <c r="C63" s="46"/>
-      <c r="D63" s="47"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="43"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -2988,7 +3044,7 @@
       <c r="F65" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G65" s="43"/>
+      <c r="G65" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="15">
@@ -3005,7 +3061,7 @@
       </c>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
-      <c r="G66" s="43"/>
+      <c r="G66" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="15">
@@ -3022,7 +3078,7 @@
       </c>
       <c r="E67" s="17"/>
       <c r="F67" s="17"/>
-      <c r="G67" s="43"/>
+      <c r="G67" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="15">
@@ -3039,7 +3095,7 @@
       </c>
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
-      <c r="G68" s="43"/>
+      <c r="G68" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="15">
@@ -3056,7 +3112,7 @@
       </c>
       <c r="E69" s="17"/>
       <c r="F69" s="17"/>
-      <c r="G69" s="43"/>
+      <c r="G69" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="15">
@@ -3073,7 +3129,7 @@
       </c>
       <c r="E70" s="17"/>
       <c r="F70" s="17"/>
-      <c r="G70" s="43"/>
+      <c r="G70" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="15">
@@ -3090,7 +3146,7 @@
       </c>
       <c r="E71" s="17"/>
       <c r="F71" s="17"/>
-      <c r="G71" s="43"/>
+      <c r="G71" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="15">
@@ -3107,7 +3163,7 @@
       </c>
       <c r="E72" s="17"/>
       <c r="F72" s="17"/>
-      <c r="G72" s="43"/>
+      <c r="G72" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="15">
@@ -3124,7 +3180,7 @@
       </c>
       <c r="E73" s="17"/>
       <c r="F73" s="17"/>
-      <c r="G73" s="43"/>
+      <c r="G73" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="15">
@@ -3141,7 +3197,7 @@
       </c>
       <c r="E74" s="17"/>
       <c r="F74" s="17"/>
-      <c r="G74" s="43"/>
+      <c r="G74" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="15">
@@ -3158,7 +3214,7 @@
       </c>
       <c r="E75" s="17"/>
       <c r="F75" s="17"/>
-      <c r="G75" s="43"/>
+      <c r="G75" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="15">
@@ -3175,16 +3231,16 @@
       </c>
       <c r="E76" s="17"/>
       <c r="F76" s="17"/>
-      <c r="G76" s="43"/>
+      <c r="G76" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="21"/>
-      <c r="B77" s="43"/>
+      <c r="B77" s="35"/>
       <c r="C77" s="30"/>
       <c r="D77" s="31"/>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
+      <c r="E77" s="35"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A78" s="11" t="s">
@@ -3216,7 +3272,7 @@
       <c r="F79" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G79" s="43"/>
+      <c r="G79" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="15">
@@ -3225,15 +3281,15 @@
       <c r="B80" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C80" s="48">
-        <v>6.120821759259259</v>
+      <c r="C80" s="44">
+        <v>9.120474537037037</v>
       </c>
       <c r="D80" s="18">
         <v>45374</v>
       </c>
       <c r="E80" s="19"/>
       <c r="F80" s="19"/>
-      <c r="G80" s="43"/>
+      <c r="G80" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="15">
@@ -3242,15 +3298,15 @@
       <c r="B81" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C81" s="48">
-        <v>6.120821759259259</v>
+      <c r="C81" s="44">
+        <v>9.120474537037037</v>
       </c>
       <c r="D81" s="18">
         <v>45375</v>
       </c>
       <c r="E81" s="19"/>
       <c r="F81" s="19"/>
-      <c r="G81" s="43"/>
+      <c r="G81" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="15">
@@ -3259,15 +3315,15 @@
       <c r="B82" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C82" s="48">
-        <v>6.120821759259259</v>
+      <c r="C82" s="44">
+        <v>9.120474537037037</v>
       </c>
       <c r="D82" s="18">
         <v>45376</v>
       </c>
       <c r="E82" s="19"/>
       <c r="F82" s="19"/>
-      <c r="G82" s="43"/>
+      <c r="G82" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="15">
@@ -3276,15 +3332,15 @@
       <c r="B83" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C83" s="48">
-        <v>6.120821759259259</v>
+      <c r="C83" s="44">
+        <v>9.120474537037037</v>
       </c>
       <c r="D83" s="18">
         <v>45377</v>
       </c>
       <c r="E83" s="19"/>
       <c r="F83" s="19"/>
-      <c r="G83" s="43"/>
+      <c r="G83" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="15">
@@ -3301,7 +3357,7 @@
       </c>
       <c r="E84" s="17"/>
       <c r="F84" s="17"/>
-      <c r="G84" s="43"/>
+      <c r="G84" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="15">
@@ -3318,7 +3374,7 @@
       </c>
       <c r="E85" s="17"/>
       <c r="F85" s="17"/>
-      <c r="G85" s="43"/>
+      <c r="G85" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="15">
@@ -3335,7 +3391,7 @@
       </c>
       <c r="E86" s="17"/>
       <c r="F86" s="17"/>
-      <c r="G86" s="43"/>
+      <c r="G86" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="15">
@@ -3352,7 +3408,7 @@
       </c>
       <c r="E87" s="17"/>
       <c r="F87" s="17"/>
-      <c r="G87" s="43"/>
+      <c r="G87" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="15">
@@ -3369,7 +3425,7 @@
       </c>
       <c r="E88" s="17"/>
       <c r="F88" s="17"/>
-      <c r="G88" s="43"/>
+      <c r="G88" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="15">
@@ -3386,7 +3442,7 @@
       </c>
       <c r="E89" s="17"/>
       <c r="F89" s="17"/>
-      <c r="G89" s="43"/>
+      <c r="G89" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="15">
@@ -3403,7 +3459,7 @@
       </c>
       <c r="E90" s="17"/>
       <c r="F90" s="17"/>
-      <c r="G90" s="43"/>
+      <c r="G90" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="15">
@@ -3420,7 +3476,7 @@
       </c>
       <c r="E91" s="17"/>
       <c r="F91" s="17"/>
-      <c r="G91" s="43"/>
+      <c r="G91" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="15">
@@ -3437,7 +3493,7 @@
       </c>
       <c r="E92" s="17"/>
       <c r="F92" s="17"/>
-      <c r="G92" s="43"/>
+      <c r="G92" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="15">
@@ -3454,7 +3510,7 @@
       </c>
       <c r="E93" s="17"/>
       <c r="F93" s="17"/>
-      <c r="G93" s="43"/>
+      <c r="G93" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="15">
@@ -3471,7 +3527,7 @@
       </c>
       <c r="E94" s="17"/>
       <c r="F94" s="17"/>
-      <c r="G94" s="43"/>
+      <c r="G94" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="15">
@@ -3488,7 +3544,7 @@
       </c>
       <c r="E95" s="17"/>
       <c r="F95" s="17"/>
-      <c r="G95" s="43"/>
+      <c r="G95" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="15">
@@ -3505,7 +3561,7 @@
       </c>
       <c r="E96" s="18"/>
       <c r="F96" s="17"/>
-      <c r="G96" s="43"/>
+      <c r="G96" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="15">
@@ -3522,7 +3578,7 @@
       </c>
       <c r="E97" s="18"/>
       <c r="F97" s="17"/>
-      <c r="G97" s="43"/>
+      <c r="G97" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="15">
@@ -3539,7 +3595,7 @@
       </c>
       <c r="E98" s="18"/>
       <c r="F98" s="17"/>
-      <c r="G98" s="43"/>
+      <c r="G98" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="15">
@@ -3556,7 +3612,7 @@
       </c>
       <c r="E99" s="18"/>
       <c r="F99" s="17"/>
-      <c r="G99" s="43"/>
+      <c r="G99" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="15">
@@ -3573,7 +3629,7 @@
       </c>
       <c r="E100" s="18"/>
       <c r="F100" s="17"/>
-      <c r="G100" s="43"/>
+      <c r="G100" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="15">
@@ -3590,7 +3646,7 @@
       </c>
       <c r="E101" s="18"/>
       <c r="F101" s="17"/>
-      <c r="G101" s="43"/>
+      <c r="G101" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="15">
@@ -3607,9 +3663,9 @@
       </c>
       <c r="E102" s="18"/>
       <c r="F102" s="17"/>
-      <c r="G102" s="43"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+      <c r="G102" s="35"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="33">
       <c r="A103" s="15">
         <v>24</v>
       </c>
@@ -3624,9 +3680,9 @@
       </c>
       <c r="E103" s="18"/>
       <c r="F103" s="17"/>
-      <c r="G103" s="43"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+      <c r="G103" s="35"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="33.75">
       <c r="A104" s="15">
         <v>25</v>
       </c>
@@ -3641,9 +3697,9 @@
       </c>
       <c r="E104" s="18"/>
       <c r="F104" s="17"/>
-      <c r="G104" s="43"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
+      <c r="G104" s="35"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="33">
       <c r="A105" s="15">
         <v>26</v>
       </c>
@@ -3658,7 +3714,7 @@
       </c>
       <c r="E105" s="18"/>
       <c r="F105" s="17"/>
-      <c r="G105" s="43"/>
+      <c r="G105" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="15">
@@ -3675,7 +3731,7 @@
       </c>
       <c r="E106" s="18"/>
       <c r="F106" s="17"/>
-      <c r="G106" s="43"/>
+      <c r="G106" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="15">
@@ -3692,9 +3748,9 @@
       </c>
       <c r="E107" s="18"/>
       <c r="F107" s="17"/>
-      <c r="G107" s="43"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
+      <c r="G107" s="35"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="33">
       <c r="A108" s="15">
         <v>29</v>
       </c>
@@ -3709,7 +3765,7 @@
       </c>
       <c r="E108" s="18"/>
       <c r="F108" s="17"/>
-      <c r="G108" s="43"/>
+      <c r="G108" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="15">
@@ -3726,850 +3782,850 @@
       </c>
       <c r="E109" s="18"/>
       <c r="F109" s="17"/>
-      <c r="G109" s="43"/>
+      <c r="G109" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="21"/>
-      <c r="B110" s="43"/>
+      <c r="B110" s="35"/>
       <c r="C110" s="30"/>
       <c r="D110" s="31"/>
-      <c r="E110" s="49"/>
-      <c r="F110" s="43"/>
-      <c r="G110" s="43"/>
+      <c r="E110" s="45"/>
+      <c r="F110" s="35"/>
+      <c r="G110" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="21"/>
-      <c r="B111" s="43"/>
+      <c r="B111" s="35"/>
       <c r="C111" s="30"/>
       <c r="D111" s="31"/>
-      <c r="E111" s="49"/>
-      <c r="F111" s="43"/>
-      <c r="G111" s="43"/>
+      <c r="E111" s="45"/>
+      <c r="F111" s="35"/>
+      <c r="G111" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="21"/>
-      <c r="B112" s="43"/>
+      <c r="B112" s="35"/>
       <c r="C112" s="30"/>
       <c r="D112" s="31"/>
-      <c r="E112" s="49"/>
-      <c r="F112" s="43"/>
-      <c r="G112" s="43"/>
+      <c r="E112" s="45"/>
+      <c r="F112" s="35"/>
+      <c r="G112" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="21"/>
-      <c r="B113" s="43"/>
+      <c r="B113" s="35"/>
       <c r="C113" s="30"/>
       <c r="D113" s="31"/>
-      <c r="E113" s="49"/>
-      <c r="F113" s="43"/>
-      <c r="G113" s="43"/>
+      <c r="E113" s="45"/>
+      <c r="F113" s="35"/>
+      <c r="G113" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="21"/>
-      <c r="B114" s="43"/>
+      <c r="B114" s="35"/>
       <c r="C114" s="30"/>
       <c r="D114" s="31"/>
-      <c r="E114" s="49"/>
-      <c r="F114" s="43"/>
-      <c r="G114" s="43"/>
+      <c r="E114" s="45"/>
+      <c r="F114" s="35"/>
+      <c r="G114" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="21"/>
-      <c r="B115" s="43"/>
+      <c r="B115" s="35"/>
       <c r="C115" s="30"/>
       <c r="D115" s="31"/>
-      <c r="E115" s="49"/>
-      <c r="F115" s="43"/>
-      <c r="G115" s="43"/>
+      <c r="E115" s="45"/>
+      <c r="F115" s="35"/>
+      <c r="G115" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="21"/>
-      <c r="B116" s="43"/>
+      <c r="B116" s="35"/>
       <c r="C116" s="30"/>
       <c r="D116" s="31"/>
-      <c r="E116" s="49"/>
-      <c r="F116" s="43"/>
-      <c r="G116" s="43"/>
+      <c r="E116" s="45"/>
+      <c r="F116" s="35"/>
+      <c r="G116" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="21"/>
-      <c r="B117" s="43"/>
+      <c r="B117" s="35"/>
       <c r="C117" s="30"/>
       <c r="D117" s="31"/>
-      <c r="E117" s="49"/>
-      <c r="F117" s="43"/>
-      <c r="G117" s="43"/>
+      <c r="E117" s="45"/>
+      <c r="F117" s="35"/>
+      <c r="G117" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="21"/>
-      <c r="B118" s="43"/>
+      <c r="B118" s="35"/>
       <c r="C118" s="30"/>
       <c r="D118" s="31"/>
-      <c r="E118" s="49"/>
-      <c r="F118" s="43"/>
-      <c r="G118" s="43"/>
+      <c r="E118" s="45"/>
+      <c r="F118" s="35"/>
+      <c r="G118" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="21"/>
-      <c r="B119" s="43"/>
+      <c r="B119" s="35"/>
       <c r="C119" s="30"/>
       <c r="D119" s="31"/>
-      <c r="E119" s="49"/>
-      <c r="F119" s="43"/>
-      <c r="G119" s="43"/>
+      <c r="E119" s="45"/>
+      <c r="F119" s="35"/>
+      <c r="G119" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="21"/>
-      <c r="B120" s="43"/>
+      <c r="B120" s="35"/>
       <c r="C120" s="30"/>
       <c r="D120" s="31"/>
-      <c r="E120" s="49"/>
-      <c r="F120" s="43"/>
-      <c r="G120" s="43"/>
+      <c r="E120" s="45"/>
+      <c r="F120" s="35"/>
+      <c r="G120" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="21"/>
-      <c r="B121" s="43"/>
+      <c r="B121" s="35"/>
       <c r="C121" s="30"/>
       <c r="D121" s="31"/>
-      <c r="E121" s="49"/>
-      <c r="F121" s="43"/>
-      <c r="G121" s="43"/>
+      <c r="E121" s="45"/>
+      <c r="F121" s="35"/>
+      <c r="G121" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="21"/>
-      <c r="B122" s="43"/>
+      <c r="B122" s="35"/>
       <c r="C122" s="30"/>
       <c r="D122" s="31"/>
-      <c r="E122" s="49"/>
-      <c r="F122" s="43"/>
-      <c r="G122" s="43"/>
+      <c r="E122" s="45"/>
+      <c r="F122" s="35"/>
+      <c r="G122" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="21"/>
-      <c r="B123" s="43"/>
+      <c r="B123" s="35"/>
       <c r="C123" s="30"/>
       <c r="D123" s="31"/>
-      <c r="E123" s="49"/>
-      <c r="F123" s="43"/>
-      <c r="G123" s="43"/>
+      <c r="E123" s="45"/>
+      <c r="F123" s="35"/>
+      <c r="G123" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="21"/>
-      <c r="B124" s="43"/>
+      <c r="B124" s="35"/>
       <c r="C124" s="30"/>
       <c r="D124" s="31"/>
-      <c r="E124" s="49"/>
-      <c r="F124" s="43"/>
-      <c r="G124" s="43"/>
+      <c r="E124" s="45"/>
+      <c r="F124" s="35"/>
+      <c r="G124" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="21"/>
-      <c r="B125" s="43"/>
+      <c r="B125" s="35"/>
       <c r="C125" s="30"/>
       <c r="D125" s="31"/>
-      <c r="E125" s="49"/>
-      <c r="F125" s="43"/>
-      <c r="G125" s="43"/>
+      <c r="E125" s="45"/>
+      <c r="F125" s="35"/>
+      <c r="G125" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="21"/>
-      <c r="B126" s="43"/>
+      <c r="B126" s="35"/>
       <c r="C126" s="30"/>
       <c r="D126" s="31"/>
-      <c r="E126" s="49"/>
-      <c r="F126" s="43"/>
-      <c r="G126" s="43"/>
+      <c r="E126" s="45"/>
+      <c r="F126" s="35"/>
+      <c r="G126" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="21"/>
-      <c r="B127" s="43"/>
+      <c r="B127" s="35"/>
       <c r="C127" s="30"/>
       <c r="D127" s="31"/>
-      <c r="E127" s="49"/>
-      <c r="F127" s="43"/>
-      <c r="G127" s="43"/>
+      <c r="E127" s="45"/>
+      <c r="F127" s="35"/>
+      <c r="G127" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="21"/>
-      <c r="B128" s="43"/>
+      <c r="B128" s="35"/>
       <c r="C128" s="30"/>
       <c r="D128" s="31"/>
-      <c r="E128" s="49"/>
-      <c r="F128" s="43"/>
-      <c r="G128" s="43"/>
+      <c r="E128" s="45"/>
+      <c r="F128" s="35"/>
+      <c r="G128" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="21"/>
-      <c r="B129" s="43"/>
+      <c r="B129" s="35"/>
       <c r="C129" s="30"/>
       <c r="D129" s="31"/>
-      <c r="E129" s="49"/>
-      <c r="F129" s="43"/>
-      <c r="G129" s="43"/>
+      <c r="E129" s="45"/>
+      <c r="F129" s="35"/>
+      <c r="G129" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="21"/>
-      <c r="B130" s="43"/>
+      <c r="B130" s="35"/>
       <c r="C130" s="30"/>
       <c r="D130" s="31"/>
-      <c r="E130" s="49"/>
-      <c r="F130" s="43"/>
-      <c r="G130" s="43"/>
+      <c r="E130" s="45"/>
+      <c r="F130" s="35"/>
+      <c r="G130" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="21"/>
-      <c r="B131" s="43"/>
+      <c r="B131" s="35"/>
       <c r="C131" s="30"/>
       <c r="D131" s="31"/>
-      <c r="E131" s="49"/>
-      <c r="F131" s="43"/>
-      <c r="G131" s="43"/>
+      <c r="E131" s="45"/>
+      <c r="F131" s="35"/>
+      <c r="G131" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="21"/>
-      <c r="B132" s="43"/>
+      <c r="B132" s="35"/>
       <c r="C132" s="30"/>
       <c r="D132" s="31"/>
-      <c r="E132" s="49"/>
-      <c r="F132" s="43"/>
-      <c r="G132" s="43"/>
+      <c r="E132" s="45"/>
+      <c r="F132" s="35"/>
+      <c r="G132" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="21"/>
-      <c r="B133" s="43"/>
+      <c r="B133" s="35"/>
       <c r="C133" s="30"/>
       <c r="D133" s="31"/>
-      <c r="E133" s="49"/>
-      <c r="F133" s="43"/>
-      <c r="G133" s="43"/>
+      <c r="E133" s="45"/>
+      <c r="F133" s="35"/>
+      <c r="G133" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="21"/>
-      <c r="B134" s="43"/>
+      <c r="B134" s="35"/>
       <c r="C134" s="30"/>
       <c r="D134" s="31"/>
-      <c r="E134" s="49"/>
-      <c r="F134" s="43"/>
-      <c r="G134" s="43"/>
+      <c r="E134" s="45"/>
+      <c r="F134" s="35"/>
+      <c r="G134" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
       <c r="A135" s="21"/>
-      <c r="B135" s="43"/>
+      <c r="B135" s="35"/>
       <c r="C135" s="30"/>
       <c r="D135" s="31"/>
-      <c r="E135" s="49"/>
-      <c r="F135" s="43"/>
-      <c r="G135" s="43"/>
+      <c r="E135" s="45"/>
+      <c r="F135" s="35"/>
+      <c r="G135" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="21"/>
-      <c r="B136" s="43"/>
+      <c r="B136" s="35"/>
       <c r="C136" s="30"/>
       <c r="D136" s="31"/>
-      <c r="E136" s="49"/>
-      <c r="F136" s="43"/>
-      <c r="G136" s="43"/>
+      <c r="E136" s="45"/>
+      <c r="F136" s="35"/>
+      <c r="G136" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="21"/>
-      <c r="B137" s="43"/>
+      <c r="B137" s="35"/>
       <c r="C137" s="30"/>
       <c r="D137" s="31"/>
-      <c r="E137" s="49"/>
-      <c r="F137" s="43"/>
-      <c r="G137" s="43"/>
+      <c r="E137" s="45"/>
+      <c r="F137" s="35"/>
+      <c r="G137" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
       <c r="A138" s="21"/>
-      <c r="B138" s="43"/>
+      <c r="B138" s="35"/>
       <c r="C138" s="30"/>
       <c r="D138" s="31"/>
-      <c r="E138" s="49"/>
-      <c r="F138" s="43"/>
-      <c r="G138" s="43"/>
+      <c r="E138" s="45"/>
+      <c r="F138" s="35"/>
+      <c r="G138" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
       <c r="A139" s="21"/>
-      <c r="B139" s="43"/>
+      <c r="B139" s="35"/>
       <c r="C139" s="30"/>
       <c r="D139" s="31"/>
-      <c r="E139" s="49"/>
-      <c r="F139" s="43"/>
-      <c r="G139" s="43"/>
+      <c r="E139" s="45"/>
+      <c r="F139" s="35"/>
+      <c r="G139" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="21"/>
-      <c r="B140" s="43"/>
+      <c r="B140" s="35"/>
       <c r="C140" s="30"/>
       <c r="D140" s="31"/>
-      <c r="E140" s="49"/>
-      <c r="F140" s="43"/>
-      <c r="G140" s="43"/>
+      <c r="E140" s="45"/>
+      <c r="F140" s="35"/>
+      <c r="G140" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
       <c r="A141" s="21"/>
-      <c r="B141" s="43"/>
+      <c r="B141" s="35"/>
       <c r="C141" s="30"/>
       <c r="D141" s="31"/>
-      <c r="E141" s="49"/>
-      <c r="F141" s="43"/>
-      <c r="G141" s="43"/>
+      <c r="E141" s="45"/>
+      <c r="F141" s="35"/>
+      <c r="G141" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
       <c r="A142" s="21"/>
-      <c r="B142" s="43"/>
+      <c r="B142" s="35"/>
       <c r="C142" s="30"/>
       <c r="D142" s="31"/>
-      <c r="E142" s="49"/>
-      <c r="F142" s="43"/>
-      <c r="G142" s="43"/>
+      <c r="E142" s="45"/>
+      <c r="F142" s="35"/>
+      <c r="G142" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="21"/>
-      <c r="B143" s="43"/>
+      <c r="B143" s="35"/>
       <c r="C143" s="30"/>
       <c r="D143" s="31"/>
-      <c r="E143" s="49"/>
-      <c r="F143" s="43"/>
-      <c r="G143" s="43"/>
+      <c r="E143" s="45"/>
+      <c r="F143" s="35"/>
+      <c r="G143" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
       <c r="A144" s="21"/>
-      <c r="B144" s="43"/>
+      <c r="B144" s="35"/>
       <c r="C144" s="30"/>
       <c r="D144" s="31"/>
-      <c r="E144" s="49"/>
-      <c r="F144" s="43"/>
-      <c r="G144" s="43"/>
+      <c r="E144" s="45"/>
+      <c r="F144" s="35"/>
+      <c r="G144" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="21"/>
-      <c r="B145" s="43"/>
+      <c r="B145" s="35"/>
       <c r="C145" s="30"/>
       <c r="D145" s="31"/>
-      <c r="E145" s="49"/>
-      <c r="F145" s="43"/>
-      <c r="G145" s="43"/>
+      <c r="E145" s="45"/>
+      <c r="F145" s="35"/>
+      <c r="G145" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="21"/>
-      <c r="B146" s="43"/>
+      <c r="B146" s="35"/>
       <c r="C146" s="30"/>
       <c r="D146" s="31"/>
-      <c r="E146" s="49"/>
-      <c r="F146" s="43"/>
-      <c r="G146" s="43"/>
+      <c r="E146" s="45"/>
+      <c r="F146" s="35"/>
+      <c r="G146" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="21"/>
-      <c r="B147" s="43"/>
+      <c r="B147" s="35"/>
       <c r="C147" s="30"/>
       <c r="D147" s="31"/>
-      <c r="E147" s="49"/>
-      <c r="F147" s="43"/>
-      <c r="G147" s="43"/>
+      <c r="E147" s="45"/>
+      <c r="F147" s="35"/>
+      <c r="G147" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="21"/>
-      <c r="B148" s="43"/>
+      <c r="B148" s="35"/>
       <c r="C148" s="30"/>
       <c r="D148" s="31"/>
-      <c r="E148" s="49"/>
-      <c r="F148" s="43"/>
-      <c r="G148" s="43"/>
+      <c r="E148" s="45"/>
+      <c r="F148" s="35"/>
+      <c r="G148" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="21"/>
-      <c r="B149" s="43"/>
+      <c r="B149" s="35"/>
       <c r="C149" s="30"/>
       <c r="D149" s="31"/>
-      <c r="E149" s="49"/>
-      <c r="F149" s="43"/>
-      <c r="G149" s="43"/>
+      <c r="E149" s="45"/>
+      <c r="F149" s="35"/>
+      <c r="G149" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
       <c r="A150" s="21"/>
-      <c r="B150" s="43"/>
+      <c r="B150" s="35"/>
       <c r="C150" s="30"/>
       <c r="D150" s="31"/>
-      <c r="E150" s="49"/>
-      <c r="F150" s="43"/>
-      <c r="G150" s="43"/>
+      <c r="E150" s="45"/>
+      <c r="F150" s="35"/>
+      <c r="G150" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="21"/>
-      <c r="B151" s="43"/>
+      <c r="B151" s="35"/>
       <c r="C151" s="30"/>
       <c r="D151" s="31"/>
-      <c r="E151" s="49"/>
-      <c r="F151" s="43"/>
-      <c r="G151" s="43"/>
+      <c r="E151" s="45"/>
+      <c r="F151" s="35"/>
+      <c r="G151" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="21"/>
-      <c r="B152" s="43"/>
+      <c r="B152" s="35"/>
       <c r="C152" s="30"/>
       <c r="D152" s="31"/>
-      <c r="E152" s="49"/>
-      <c r="F152" s="43"/>
-      <c r="G152" s="43"/>
+      <c r="E152" s="45"/>
+      <c r="F152" s="35"/>
+      <c r="G152" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="21"/>
-      <c r="B153" s="43"/>
+      <c r="B153" s="35"/>
       <c r="C153" s="30"/>
       <c r="D153" s="31"/>
-      <c r="E153" s="49"/>
-      <c r="F153" s="43"/>
-      <c r="G153" s="43"/>
+      <c r="E153" s="45"/>
+      <c r="F153" s="35"/>
+      <c r="G153" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="21"/>
-      <c r="B154" s="43"/>
+      <c r="B154" s="35"/>
       <c r="C154" s="30"/>
       <c r="D154" s="31"/>
-      <c r="E154" s="49"/>
-      <c r="F154" s="43"/>
-      <c r="G154" s="43"/>
+      <c r="E154" s="45"/>
+      <c r="F154" s="35"/>
+      <c r="G154" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="21"/>
-      <c r="B155" s="43"/>
+      <c r="B155" s="35"/>
       <c r="C155" s="30"/>
       <c r="D155" s="31"/>
-      <c r="E155" s="49"/>
-      <c r="F155" s="43"/>
-      <c r="G155" s="43"/>
+      <c r="E155" s="45"/>
+      <c r="F155" s="35"/>
+      <c r="G155" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="21"/>
-      <c r="B156" s="43"/>
+      <c r="B156" s="35"/>
       <c r="C156" s="30"/>
       <c r="D156" s="31"/>
-      <c r="E156" s="49"/>
-      <c r="F156" s="43"/>
-      <c r="G156" s="43"/>
+      <c r="E156" s="45"/>
+      <c r="F156" s="35"/>
+      <c r="G156" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="21"/>
-      <c r="B157" s="43"/>
+      <c r="B157" s="35"/>
       <c r="C157" s="30"/>
       <c r="D157" s="31"/>
-      <c r="E157" s="49"/>
-      <c r="F157" s="43"/>
-      <c r="G157" s="43"/>
+      <c r="E157" s="45"/>
+      <c r="F157" s="35"/>
+      <c r="G157" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="21"/>
-      <c r="B158" s="43"/>
+      <c r="B158" s="35"/>
       <c r="C158" s="30"/>
       <c r="D158" s="31"/>
-      <c r="E158" s="49"/>
-      <c r="F158" s="43"/>
-      <c r="G158" s="43"/>
+      <c r="E158" s="45"/>
+      <c r="F158" s="35"/>
+      <c r="G158" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="21"/>
-      <c r="B159" s="43"/>
+      <c r="B159" s="35"/>
       <c r="C159" s="30"/>
       <c r="D159" s="31"/>
-      <c r="E159" s="49"/>
-      <c r="F159" s="43"/>
-      <c r="G159" s="43"/>
+      <c r="E159" s="45"/>
+      <c r="F159" s="35"/>
+      <c r="G159" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="21"/>
-      <c r="B160" s="43"/>
+      <c r="B160" s="35"/>
       <c r="C160" s="30"/>
       <c r="D160" s="31"/>
-      <c r="E160" s="49"/>
-      <c r="F160" s="43"/>
-      <c r="G160" s="43"/>
+      <c r="E160" s="45"/>
+      <c r="F160" s="35"/>
+      <c r="G160" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="21"/>
-      <c r="B161" s="43"/>
+      <c r="B161" s="35"/>
       <c r="C161" s="30"/>
       <c r="D161" s="31"/>
-      <c r="E161" s="49"/>
-      <c r="F161" s="43"/>
-      <c r="G161" s="43"/>
+      <c r="E161" s="45"/>
+      <c r="F161" s="35"/>
+      <c r="G161" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="21"/>
-      <c r="B162" s="43"/>
+      <c r="B162" s="35"/>
       <c r="C162" s="30"/>
       <c r="D162" s="31"/>
-      <c r="E162" s="49"/>
-      <c r="F162" s="43"/>
-      <c r="G162" s="43"/>
+      <c r="E162" s="45"/>
+      <c r="F162" s="35"/>
+      <c r="G162" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="21"/>
-      <c r="B163" s="43"/>
+      <c r="B163" s="35"/>
       <c r="C163" s="30"/>
       <c r="D163" s="31"/>
-      <c r="E163" s="49"/>
-      <c r="F163" s="43"/>
-      <c r="G163" s="43"/>
+      <c r="E163" s="45"/>
+      <c r="F163" s="35"/>
+      <c r="G163" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="21"/>
-      <c r="B164" s="43"/>
+      <c r="B164" s="35"/>
       <c r="C164" s="30"/>
       <c r="D164" s="31"/>
-      <c r="E164" s="49"/>
-      <c r="F164" s="43"/>
-      <c r="G164" s="43"/>
+      <c r="E164" s="45"/>
+      <c r="F164" s="35"/>
+      <c r="G164" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="21"/>
-      <c r="B165" s="43"/>
+      <c r="B165" s="35"/>
       <c r="C165" s="30"/>
       <c r="D165" s="31"/>
-      <c r="E165" s="49"/>
-      <c r="F165" s="43"/>
-      <c r="G165" s="43"/>
+      <c r="E165" s="45"/>
+      <c r="F165" s="35"/>
+      <c r="G165" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
       <c r="A166" s="21"/>
-      <c r="B166" s="43"/>
+      <c r="B166" s="35"/>
       <c r="C166" s="30"/>
       <c r="D166" s="31"/>
-      <c r="E166" s="49"/>
-      <c r="F166" s="43"/>
-      <c r="G166" s="43"/>
+      <c r="E166" s="45"/>
+      <c r="F166" s="35"/>
+      <c r="G166" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="21"/>
-      <c r="B167" s="43"/>
+      <c r="B167" s="35"/>
       <c r="C167" s="30"/>
       <c r="D167" s="31"/>
-      <c r="E167" s="49"/>
-      <c r="F167" s="43"/>
-      <c r="G167" s="43"/>
+      <c r="E167" s="45"/>
+      <c r="F167" s="35"/>
+      <c r="G167" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
       <c r="A168" s="21"/>
-      <c r="B168" s="43"/>
+      <c r="B168" s="35"/>
       <c r="C168" s="30"/>
       <c r="D168" s="31"/>
-      <c r="E168" s="49"/>
-      <c r="F168" s="43"/>
-      <c r="G168" s="43"/>
+      <c r="E168" s="45"/>
+      <c r="F168" s="35"/>
+      <c r="G168" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
       <c r="A169" s="21"/>
-      <c r="B169" s="43"/>
+      <c r="B169" s="35"/>
       <c r="C169" s="30"/>
       <c r="D169" s="31"/>
-      <c r="E169" s="49"/>
-      <c r="F169" s="43"/>
-      <c r="G169" s="43"/>
+      <c r="E169" s="45"/>
+      <c r="F169" s="35"/>
+      <c r="G169" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
       <c r="A170" s="21"/>
-      <c r="B170" s="43"/>
+      <c r="B170" s="35"/>
       <c r="C170" s="30"/>
       <c r="D170" s="31"/>
-      <c r="E170" s="49"/>
-      <c r="F170" s="43"/>
-      <c r="G170" s="43"/>
+      <c r="E170" s="45"/>
+      <c r="F170" s="35"/>
+      <c r="G170" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="21"/>
-      <c r="B171" s="43"/>
+      <c r="B171" s="35"/>
       <c r="C171" s="30"/>
       <c r="D171" s="31"/>
-      <c r="E171" s="49"/>
-      <c r="F171" s="43"/>
-      <c r="G171" s="43"/>
+      <c r="E171" s="45"/>
+      <c r="F171" s="35"/>
+      <c r="G171" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
       <c r="A172" s="21"/>
-      <c r="B172" s="43"/>
+      <c r="B172" s="35"/>
       <c r="C172" s="30"/>
       <c r="D172" s="31"/>
-      <c r="E172" s="49"/>
-      <c r="F172" s="43"/>
-      <c r="G172" s="43"/>
+      <c r="E172" s="45"/>
+      <c r="F172" s="35"/>
+      <c r="G172" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
       <c r="A173" s="21"/>
-      <c r="B173" s="43"/>
+      <c r="B173" s="35"/>
       <c r="C173" s="30"/>
       <c r="D173" s="31"/>
-      <c r="E173" s="49"/>
-      <c r="F173" s="43"/>
-      <c r="G173" s="43"/>
+      <c r="E173" s="45"/>
+      <c r="F173" s="35"/>
+      <c r="G173" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="21"/>
-      <c r="B174" s="43"/>
+      <c r="B174" s="35"/>
       <c r="C174" s="30"/>
       <c r="D174" s="31"/>
-      <c r="E174" s="49"/>
-      <c r="F174" s="43"/>
-      <c r="G174" s="43"/>
+      <c r="E174" s="45"/>
+      <c r="F174" s="35"/>
+      <c r="G174" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="21"/>
-      <c r="B175" s="43"/>
+      <c r="B175" s="35"/>
       <c r="C175" s="30"/>
       <c r="D175" s="31"/>
-      <c r="E175" s="49"/>
-      <c r="F175" s="43"/>
-      <c r="G175" s="43"/>
+      <c r="E175" s="45"/>
+      <c r="F175" s="35"/>
+      <c r="G175" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
       <c r="A176" s="21"/>
       <c r="B176" s="2"/>
-      <c r="C176" s="50"/>
+      <c r="C176" s="46"/>
       <c r="D176" s="31"/>
-      <c r="E176" s="43"/>
-      <c r="F176" s="43"/>
-      <c r="G176" s="43"/>
+      <c r="E176" s="35"/>
+      <c r="F176" s="35"/>
+      <c r="G176" s="35"/>
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A177" s="45"/>
+      <c r="A177" s="41"/>
       <c r="B177" s="2"/>
-      <c r="C177" s="46"/>
-      <c r="D177" s="47"/>
+      <c r="C177" s="42"/>
+      <c r="D177" s="43"/>
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
       <c r="G177" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A178" s="45"/>
+      <c r="A178" s="41"/>
       <c r="B178" s="2"/>
-      <c r="C178" s="46"/>
-      <c r="D178" s="47"/>
+      <c r="C178" s="42"/>
+      <c r="D178" s="43"/>
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A179" s="45"/>
+      <c r="A179" s="41"/>
       <c r="B179" s="2"/>
-      <c r="C179" s="46"/>
-      <c r="D179" s="47"/>
+      <c r="C179" s="42"/>
+      <c r="D179" s="43"/>
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
       <c r="G179" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A180" s="45"/>
+      <c r="A180" s="41"/>
       <c r="B180" s="2"/>
-      <c r="C180" s="46"/>
-      <c r="D180" s="47"/>
+      <c r="C180" s="42"/>
+      <c r="D180" s="43"/>
       <c r="E180" s="2"/>
       <c r="F180" s="2"/>
       <c r="G180" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A181" s="45"/>
+      <c r="A181" s="41"/>
       <c r="B181" s="2"/>
-      <c r="C181" s="46"/>
-      <c r="D181" s="47"/>
+      <c r="C181" s="42"/>
+      <c r="D181" s="43"/>
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
       <c r="G181" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A182" s="45"/>
+      <c r="A182" s="41"/>
       <c r="B182" s="2"/>
-      <c r="C182" s="46"/>
-      <c r="D182" s="47"/>
+      <c r="C182" s="42"/>
+      <c r="D182" s="43"/>
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
       <c r="G182" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A183" s="45"/>
+      <c r="A183" s="41"/>
       <c r="B183" s="2"/>
-      <c r="C183" s="46"/>
-      <c r="D183" s="47"/>
+      <c r="C183" s="42"/>
+      <c r="D183" s="43"/>
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
       <c r="G183" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A184" s="45"/>
+      <c r="A184" s="41"/>
       <c r="B184" s="2"/>
-      <c r="C184" s="46"/>
-      <c r="D184" s="47"/>
+      <c r="C184" s="42"/>
+      <c r="D184" s="43"/>
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A185" s="45"/>
+      <c r="A185" s="41"/>
       <c r="B185" s="2"/>
-      <c r="C185" s="46"/>
-      <c r="D185" s="47"/>
+      <c r="C185" s="42"/>
+      <c r="D185" s="43"/>
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A186" s="45"/>
+      <c r="A186" s="41"/>
       <c r="B186" s="2"/>
-      <c r="C186" s="46"/>
-      <c r="D186" s="47"/>
+      <c r="C186" s="42"/>
+      <c r="D186" s="43"/>
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A187" s="45"/>
+      <c r="A187" s="41"/>
       <c r="B187" s="2"/>
-      <c r="C187" s="46"/>
-      <c r="D187" s="47"/>
+      <c r="C187" s="42"/>
+      <c r="D187" s="43"/>
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A188" s="45"/>
+      <c r="A188" s="41"/>
       <c r="B188" s="2"/>
-      <c r="C188" s="46"/>
-      <c r="D188" s="47"/>
+      <c r="C188" s="42"/>
+      <c r="D188" s="43"/>
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A189" s="45"/>
+      <c r="A189" s="41"/>
       <c r="B189" s="2"/>
-      <c r="C189" s="46"/>
-      <c r="D189" s="47"/>
+      <c r="C189" s="42"/>
+      <c r="D189" s="43"/>
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
       <c r="G189" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A190" s="45"/>
+      <c r="A190" s="41"/>
       <c r="B190" s="2"/>
-      <c r="C190" s="46"/>
-      <c r="D190" s="47"/>
+      <c r="C190" s="42"/>
+      <c r="D190" s="43"/>
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
       <c r="G190" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A191" s="45"/>
+      <c r="A191" s="41"/>
       <c r="B191" s="2"/>
-      <c r="C191" s="46"/>
-      <c r="D191" s="47"/>
+      <c r="C191" s="42"/>
+      <c r="D191" s="43"/>
       <c r="E191" s="2"/>
       <c r="F191" s="2"/>
       <c r="G191" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A192" s="45"/>
+      <c r="A192" s="41"/>
       <c r="B192" s="2"/>
-      <c r="C192" s="46"/>
-      <c r="D192" s="47"/>
+      <c r="C192" s="42"/>
+      <c r="D192" s="43"/>
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
       <c r="G192" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A193" s="45"/>
+      <c r="A193" s="41"/>
       <c r="B193" s="2"/>
-      <c r="C193" s="46"/>
-      <c r="D193" s="47"/>
+      <c r="C193" s="42"/>
+      <c r="D193" s="43"/>
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A194" s="45"/>
+      <c r="A194" s="41"/>
       <c r="B194" s="2"/>
-      <c r="C194" s="46"/>
-      <c r="D194" s="47"/>
+      <c r="C194" s="42"/>
+      <c r="D194" s="43"/>
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A195" s="45"/>
+      <c r="A195" s="41"/>
       <c r="B195" s="2"/>
-      <c r="C195" s="46"/>
-      <c r="D195" s="47"/>
+      <c r="C195" s="42"/>
+      <c r="D195" s="43"/>
       <c r="E195" s="2"/>
       <c r="F195" s="2"/>
       <c r="G195" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A196" s="45"/>
+      <c r="A196" s="41"/>
       <c r="B196" s="2"/>
-      <c r="C196" s="46"/>
-      <c r="D196" s="47"/>
+      <c r="C196" s="42"/>
+      <c r="D196" s="43"/>
       <c r="E196" s="2"/>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A197" s="45"/>
+      <c r="A197" s="41"/>
       <c r="B197" s="2"/>
-      <c r="C197" s="46"/>
-      <c r="D197" s="47"/>
+      <c r="C197" s="42"/>
+      <c r="D197" s="43"/>
       <c r="E197" s="2"/>
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A198" s="45"/>
+      <c r="A198" s="41"/>
       <c r="B198" s="2"/>
-      <c r="C198" s="46"/>
-      <c r="D198" s="47"/>
+      <c r="C198" s="42"/>
+      <c r="D198" s="43"/>
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
       <c r="G198" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A199" s="45"/>
+      <c r="A199" s="41"/>
       <c r="B199" s="2"/>
-      <c r="C199" s="46"/>
-      <c r="D199" s="47"/>
+      <c r="C199" s="42"/>
+      <c r="D199" s="43"/>
       <c r="E199" s="2"/>
       <c r="F199" s="2"/>
       <c r="G199" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A200" s="45"/>
+      <c r="A200" s="41"/>
       <c r="B200" s="2"/>
-      <c r="C200" s="46"/>
-      <c r="D200" s="47"/>
+      <c r="C200" s="42"/>
+      <c r="D200" s="43"/>
       <c r="E200" s="2"/>
       <c r="F200" s="2"/>
       <c r="G200" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A201" s="45"/>
+      <c r="A201" s="41"/>
       <c r="B201" s="2"/>
-      <c r="C201" s="46"/>
-      <c r="D201" s="47"/>
+      <c r="C201" s="42"/>
+      <c r="D201" s="43"/>
       <c r="E201" s="2"/>
       <c r="F201" s="2"/>
       <c r="G201" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A202" s="45"/>
+      <c r="A202" s="41"/>
       <c r="B202" s="2"/>
-      <c r="C202" s="46"/>
-      <c r="D202" s="47"/>
+      <c r="C202" s="42"/>
+      <c r="D202" s="43"/>
       <c r="E202" s="2"/>
       <c r="F202" s="2"/>
       <c r="G202" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A203" s="45"/>
+      <c r="A203" s="41"/>
       <c r="B203" s="2"/>
-      <c r="C203" s="46"/>
-      <c r="D203" s="47"/>
+      <c r="C203" s="42"/>
+      <c r="D203" s="43"/>
       <c r="E203" s="2"/>
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>

</xml_diff>

<commit_message>
few more JS programs
</commit_message>
<xml_diff>
--- a/001EffortTracker/KT Plan.xlsx
+++ b/001EffortTracker/KT Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Index"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="340">
   <si>
     <t>Playwright: Web Automation Testing From Zero to Hero - Artem Bondar</t>
   </si>
@@ -594,8 +594,7 @@
     <t>Revise previous days topics Next days - find a way to achive this</t>
   </si>
   <si>
-    <t>Practise more programs outside the course aswel, 
-Generate your own programs and scenarios and try to implement it</t>
+    <t>Practise more programs outside the course aswel, Generate your own programs and scenarios and try to implement it</t>
   </si>
   <si>
     <t>JavaScript - YouTube - NaveenAutoLabs</t>
@@ -2088,13 +2087,13 @@
   </sheetPr>
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="23" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="23" width="7.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="47" width="60.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="33" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="33" width="10.862142857142858" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="34" width="7.719285714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="47" width="12.005" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="47" width="15.43357142857143" customWidth="1" bestFit="1"/>
@@ -2138,7 +2137,7 @@
       <c r="F3" s="35"/>
       <c r="G3" s="35"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -2530,7 +2529,9 @@
       <c r="D25" s="18">
         <v>45361</v>
       </c>
-      <c r="E25" s="17"/>
+      <c r="E25" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F25" s="17" t="s">
         <v>212</v>
       </c>
@@ -2549,7 +2550,9 @@
       <c r="D26" s="18">
         <v>45361</v>
       </c>
-      <c r="E26" s="17"/>
+      <c r="E26" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F26" s="17" t="s">
         <v>212</v>
       </c>
@@ -2568,7 +2571,9 @@
       <c r="D27" s="18">
         <v>45362</v>
       </c>
-      <c r="E27" s="17"/>
+      <c r="E27" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F27" s="17" t="s">
         <v>215</v>
       </c>
@@ -2587,7 +2592,9 @@
       <c r="D28" s="18">
         <v>45362</v>
       </c>
-      <c r="E28" s="17"/>
+      <c r="E28" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F28" s="17" t="s">
         <v>215</v>
       </c>
@@ -2669,7 +2676,7 @@
       </c>
       <c r="G32" s="35"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="15">
         <v>26</v>
       </c>
@@ -3522,7 +3529,7 @@
         <v>272</v>
       </c>
       <c r="C80" s="44">
-        <v>12.120127314814814</v>
+        <v>14.119895833333333</v>
       </c>
       <c r="D80" s="18">
         <v>45374</v>
@@ -3541,7 +3548,7 @@
         <v>272</v>
       </c>
       <c r="C81" s="44">
-        <v>12.120127314814814</v>
+        <v>14.119895833333333</v>
       </c>
       <c r="D81" s="18">
         <v>45375</v>
@@ -3560,7 +3567,7 @@
         <v>272</v>
       </c>
       <c r="C82" s="44">
-        <v>12.120127314814814</v>
+        <v>14.119895833333333</v>
       </c>
       <c r="D82" s="18">
         <v>45376</v>
@@ -3579,7 +3586,7 @@
         <v>272</v>
       </c>
       <c r="C83" s="44">
-        <v>12.120127314814814</v>
+        <v>14.119895833333333</v>
       </c>
       <c r="D83" s="18">
         <v>45377</v>
@@ -4948,7 +4955,7 @@
   </sheetPr>
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
promise, promiseChain, promiseAll, promiseAllSettled, promiseRace, promiseAny
</commit_message>
<xml_diff>
--- a/001EffortTracker/KT Plan.xlsx
+++ b/001EffortTracker/KT Plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="340">
   <si>
     <t>Playwright: Web Automation Testing From Zero to Hero - Artem Bondar</t>
   </si>
@@ -2111,7 +2111,7 @@
       <c r="F1" s="35"/>
       <c r="G1" s="35"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="47.25">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="G7" s="35"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33.75">
       <c r="A8" s="15">
         <v>1</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>196</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="33.75">
       <c r="A11" s="15">
         <v>4</v>
       </c>
@@ -2613,7 +2613,9 @@
       <c r="D29" s="18">
         <v>45362</v>
       </c>
-      <c r="E29" s="17"/>
+      <c r="E29" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F29" s="17" t="s">
         <v>215</v>
       </c>
@@ -2632,7 +2634,9 @@
       <c r="D30" s="18">
         <v>45362</v>
       </c>
-      <c r="E30" s="17"/>
+      <c r="E30" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F30" s="17" t="s">
         <v>215</v>
       </c>
@@ -2651,7 +2655,9 @@
       <c r="D31" s="18">
         <v>45363</v>
       </c>
-      <c r="E31" s="17"/>
+      <c r="E31" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F31" s="17" t="s">
         <v>220</v>
       </c>
@@ -2670,7 +2676,9 @@
       <c r="D32" s="18">
         <v>45363</v>
       </c>
-      <c r="E32" s="17"/>
+      <c r="E32" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F32" s="17" t="s">
         <v>220</v>
       </c>
@@ -2689,7 +2697,9 @@
       <c r="D33" s="18">
         <v>45363</v>
       </c>
-      <c r="E33" s="17"/>
+      <c r="E33" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F33" s="17" t="s">
         <v>220</v>
       </c>
@@ -2708,7 +2718,9 @@
       <c r="D34" s="18">
         <v>45363</v>
       </c>
-      <c r="E34" s="17"/>
+      <c r="E34" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="F34" s="17" t="s">
         <v>220</v>
       </c>
@@ -3529,7 +3541,7 @@
         <v>272</v>
       </c>
       <c r="C80" s="44">
-        <v>14.119895833333333</v>
+        <v>15.119780092592592</v>
       </c>
       <c r="D80" s="18">
         <v>45374</v>
@@ -3548,7 +3560,7 @@
         <v>272</v>
       </c>
       <c r="C81" s="44">
-        <v>14.119895833333333</v>
+        <v>15.119780092592592</v>
       </c>
       <c r="D81" s="18">
         <v>45375</v>
@@ -3567,7 +3579,7 @@
         <v>272</v>
       </c>
       <c r="C82" s="44">
-        <v>14.119895833333333</v>
+        <v>15.119780092592592</v>
       </c>
       <c r="D82" s="18">
         <v>45376</v>
@@ -3586,7 +3598,7 @@
         <v>272</v>
       </c>
       <c r="C83" s="44">
-        <v>14.119895833333333</v>
+        <v>15.119780092592592</v>
       </c>
       <c r="D83" s="18">
         <v>45377</v>

</xml_diff>

<commit_message>
promiseChaining and async&await concepts
</commit_message>
<xml_diff>
--- a/001EffortTracker/KT Plan.xlsx
+++ b/001EffortTracker/KT Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Index"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="343">
   <si>
     <t>Playwright: Web Automation Testing From Zero to Hero - Artem Bondar</t>
   </si>
@@ -1047,6 +1047,12 @@
   <si>
     <t>https://www.lambdatest.com/certifications/playwright-101
 https://www.vskills.in/certification/playwright-certification-course</t>
+  </si>
+  <si>
+    <t>JavaScript &amp; Node.js course for Testers, QA and SDETs - 2024</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/javascript-and-nodejs-essentials-for-test-automation</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1622,7 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2048,15 +2054,25 @@
         <v>340</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="40.5">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
+      <c r="D24" s="48">
+        <v>22</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="F24" s="21">
+        <v>1</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>319</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="22"/>
@@ -2090,7 +2106,7 @@
   </sheetPr>
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>